<commit_message>
Some changes and table calculations
</commit_message>
<xml_diff>
--- a/readme/XJDF Format Mappings.xlsx
+++ b/readme/XJDF Format Mappings.xlsx
@@ -4,19 +4,20 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-4800" yWindow="1170" windowWidth="24915" windowHeight="14130" activeTab="1"/>
+    <workbookView xWindow="-4800" yWindow="1170" windowWidth="24915" windowHeight="14130" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Paragraph" sheetId="1" r:id="rId1"/>
     <sheet name="Character" sheetId="2" r:id="rId2"/>
     <sheet name="Cross Ref" sheetId="3" r:id="rId3"/>
+    <sheet name="Table widths" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="448" uniqueCount="271">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="461" uniqueCount="281">
   <si>
     <t>AnchorFigure</t>
   </si>
@@ -829,6 +830,36 @@
   </si>
   <si>
     <t>All become "Example X.Y ShowingOff"</t>
+  </si>
+  <si>
+    <t>Page Width</t>
+  </si>
+  <si>
+    <t>mm</t>
+  </si>
+  <si>
+    <t>Flow Width</t>
+  </si>
+  <si>
+    <t>Margins</t>
+  </si>
+  <si>
+    <t>Inches</t>
+  </si>
+  <si>
+    <t>Points</t>
+  </si>
+  <si>
+    <t>FM Value</t>
+  </si>
+  <si>
+    <t>Column 1</t>
+  </si>
+  <si>
+    <t>Column 2</t>
+  </si>
+  <si>
+    <t>Column 3</t>
   </si>
 </sst>
 </file>
@@ -1125,7 +1156,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -1154,6 +1185,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1453,8 +1485,8 @@
   </sheetPr>
   <dimension ref="B3:E84"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="A35" sqref="A35"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B64" sqref="B64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2411,8 +2443,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B3:E53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2494,9 +2526,7 @@
       <c r="B10" s="11" t="s">
         <v>104</v>
       </c>
-      <c r="C10" s="12" t="s">
-        <v>104</v>
-      </c>
+      <c r="C10" s="12"/>
       <c r="D10" s="12" t="s">
         <v>151</v>
       </c>
@@ -2755,12 +2785,14 @@
       </c>
     </row>
     <row r="34" spans="2:5">
-      <c r="B34" s="5" t="s">
+      <c r="B34" s="11" t="s">
         <v>128</v>
       </c>
-      <c r="C34" s="6"/>
-      <c r="D34" s="6"/>
-      <c r="E34" s="7" t="s">
+      <c r="C34" s="12" t="s">
+        <v>128</v>
+      </c>
+      <c r="D34" s="12"/>
+      <c r="E34" s="13" t="s">
         <v>233</v>
       </c>
     </row>
@@ -2904,7 +2936,9 @@
       <c r="B47" s="5" t="s">
         <v>141</v>
       </c>
-      <c r="C47" s="6"/>
+      <c r="C47" s="6" t="s">
+        <v>140</v>
+      </c>
       <c r="D47" s="6"/>
       <c r="E47" s="7" t="s">
         <v>226</v>
@@ -2924,7 +2958,9 @@
       <c r="B49" s="5" t="s">
         <v>143</v>
       </c>
-      <c r="C49" s="6"/>
+      <c r="C49" s="6" t="s">
+        <v>142</v>
+      </c>
       <c r="D49" s="6"/>
       <c r="E49" s="7" t="s">
         <v>227</v>
@@ -2944,7 +2980,9 @@
       <c r="B51" s="11" t="s">
         <v>145</v>
       </c>
-      <c r="C51" s="12"/>
+      <c r="C51" s="6" t="s">
+        <v>144</v>
+      </c>
       <c r="D51" s="12"/>
       <c r="E51" s="13" t="s">
         <v>152</v>
@@ -3437,4 +3475,169 @@
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="C2:K12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M6" sqref="M6:M8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="11" max="11" width="9.5703125" style="28" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="3:11">
+      <c r="G2">
+        <v>25.4</v>
+      </c>
+      <c r="I2">
+        <v>72</v>
+      </c>
+      <c r="K2" s="28">
+        <v>65536</v>
+      </c>
+    </row>
+    <row r="3" spans="3:11">
+      <c r="E3" t="s">
+        <v>272</v>
+      </c>
+      <c r="G3" t="s">
+        <v>275</v>
+      </c>
+      <c r="I3" t="s">
+        <v>276</v>
+      </c>
+      <c r="K3" s="28" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="4" spans="3:11">
+      <c r="C4" t="s">
+        <v>271</v>
+      </c>
+      <c r="E4">
+        <v>210</v>
+      </c>
+      <c r="G4">
+        <f>E4/$G$2</f>
+        <v>8.2677165354330722</v>
+      </c>
+      <c r="I4">
+        <f>G4*$I$2</f>
+        <v>595.27559055118115</v>
+      </c>
+      <c r="K4" s="28">
+        <f>I4*$K$2</f>
+        <v>39011981.102362208</v>
+      </c>
+    </row>
+    <row r="6" spans="3:11">
+      <c r="C6" t="s">
+        <v>274</v>
+      </c>
+      <c r="E6">
+        <v>12</v>
+      </c>
+      <c r="G6">
+        <f>E6/$G$2</f>
+        <v>0.47244094488188981</v>
+      </c>
+      <c r="I6">
+        <f>G6*$I$2</f>
+        <v>34.015748031496067</v>
+      </c>
+      <c r="K6" s="28">
+        <f>I6*$K$2</f>
+        <v>2229256.0629921262</v>
+      </c>
+    </row>
+    <row r="8" spans="3:11">
+      <c r="C8" t="s">
+        <v>273</v>
+      </c>
+      <c r="E8">
+        <f>E4-(2*E6)</f>
+        <v>186</v>
+      </c>
+      <c r="G8">
+        <f>E8/$G$2</f>
+        <v>7.3228346456692917</v>
+      </c>
+      <c r="I8">
+        <f>G8*$I$2</f>
+        <v>527.24409448818903</v>
+      </c>
+      <c r="K8" s="28">
+        <f>I8*$K$2</f>
+        <v>34553468.976377957</v>
+      </c>
+    </row>
+    <row r="10" spans="3:11">
+      <c r="C10" t="s">
+        <v>278</v>
+      </c>
+      <c r="E10">
+        <v>35</v>
+      </c>
+      <c r="G10">
+        <f t="shared" ref="G10:G12" si="0">E10/$G$2</f>
+        <v>1.3779527559055118</v>
+      </c>
+      <c r="I10">
+        <f t="shared" ref="I10:I12" si="1">G10*$I$2</f>
+        <v>99.212598425196845</v>
+      </c>
+      <c r="K10" s="28">
+        <f>I10*$K$2</f>
+        <v>6501996.8503937004</v>
+      </c>
+    </row>
+    <row r="11" spans="3:11">
+      <c r="C11" t="s">
+        <v>279</v>
+      </c>
+      <c r="E11">
+        <v>26</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="0"/>
+        <v>1.0236220472440944</v>
+      </c>
+      <c r="I11">
+        <f t="shared" si="1"/>
+        <v>73.7007874015748</v>
+      </c>
+      <c r="K11" s="28">
+        <f>I11*$K$2</f>
+        <v>4830054.8031496061</v>
+      </c>
+    </row>
+    <row r="12" spans="3:11">
+      <c r="C12" t="s">
+        <v>280</v>
+      </c>
+      <c r="E12">
+        <f>E8-E10-E11</f>
+        <v>125</v>
+      </c>
+      <c r="G12">
+        <f t="shared" si="0"/>
+        <v>4.9212598425196852</v>
+      </c>
+      <c r="I12">
+        <f t="shared" si="1"/>
+        <v>354.33070866141736</v>
+      </c>
+      <c r="K12" s="28">
+        <f>I12*$K$2</f>
+        <v>23221417.322834648</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Update to the mapping required for migrating to V5 format
</commit_message>
<xml_diff>
--- a/readme/XJDF Format Mappings.xlsx
+++ b/readme/XJDF Format Mappings.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-4800" yWindow="1170" windowWidth="24915" windowHeight="14130" activeTab="3"/>
+    <workbookView xWindow="-4800" yWindow="1170" windowWidth="24915" windowHeight="14130"/>
   </bookViews>
   <sheets>
     <sheet name="Paragraph" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="461" uniqueCount="281">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="469" uniqueCount="287">
   <si>
     <t>AnchorFigure</t>
   </si>
@@ -466,9 +466,6 @@
     <t>Emphasis</t>
   </si>
   <si>
-    <t>Was used to prevent spelling.</t>
-  </si>
-  <si>
     <t>Confirm removal Ok</t>
   </si>
   <si>
@@ -860,12 +857,36 @@
   </si>
   <si>
     <t>Column 3</t>
+  </si>
+  <si>
+    <t>Was used to prevent spelling - mostly on attribute/element cardinality symbols.</t>
+  </si>
+  <si>
+    <t>General page layout</t>
+  </si>
+  <si>
+    <t>Column1</t>
+  </si>
+  <si>
+    <t>JMF, Resources, Subelements</t>
+  </si>
+  <si>
+    <t>All Tables that are one column wide get the full flow width - regardless of the document (JMF, Resources, Appx etc)</t>
+  </si>
+  <si>
+    <t>Processes (I/O Resource Tables are two columns)</t>
+  </si>
+  <si>
+    <t>Check!</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="1">
+    <numFmt numFmtId="166" formatCode="0.00000"/>
+  </numFmts>
   <fonts count="2">
     <font>
       <sz val="11"/>
@@ -1156,7 +1177,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -1186,6 +1207,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1485,7 +1507,7 @@
   </sheetPr>
   <dimension ref="B3:E84"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
       <selection activeCell="B64" sqref="B64"/>
     </sheetView>
   </sheetViews>
@@ -1534,7 +1556,7 @@
       </c>
       <c r="D6" s="6"/>
       <c r="E6" s="7" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="7" spans="2:5">
@@ -1620,7 +1642,7 @@
       </c>
       <c r="D14" s="9"/>
       <c r="E14" s="10" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="15" spans="2:5">
@@ -1632,7 +1654,7 @@
       </c>
       <c r="D15" s="12"/>
       <c r="E15" s="13" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="16" spans="2:5">
@@ -1644,7 +1666,7 @@
       </c>
       <c r="D16" s="12"/>
       <c r="E16" s="13" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="17" spans="2:5">
@@ -1656,7 +1678,7 @@
       </c>
       <c r="D17" s="12"/>
       <c r="E17" s="13" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="18" spans="2:5">
@@ -1716,7 +1738,7 @@
       </c>
       <c r="D22" s="15"/>
       <c r="E22" s="16" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="23" spans="2:5">
@@ -1728,7 +1750,7 @@
       </c>
       <c r="D23" s="9"/>
       <c r="E23" s="10" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="24" spans="2:5">
@@ -1790,12 +1812,12 @@
         <v>85</v>
       </c>
       <c r="E28" s="7" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="29" spans="2:5">
       <c r="B29" s="5" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C29" s="6" t="s">
         <v>19</v>
@@ -1804,12 +1826,12 @@
         <v>84</v>
       </c>
       <c r="E29" s="7" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="30" spans="2:5">
       <c r="B30" s="5" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C30" s="6" t="s">
         <v>19</v>
@@ -1818,12 +1840,12 @@
         <v>84</v>
       </c>
       <c r="E30" s="7" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="31" spans="2:5">
       <c r="B31" s="5" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C31" s="6" t="s">
         <v>19</v>
@@ -1832,7 +1854,7 @@
         <v>84</v>
       </c>
       <c r="E31" s="7" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="32" spans="2:5">
@@ -1849,7 +1871,7 @@
     </row>
     <row r="33" spans="2:5">
       <c r="B33" s="5" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C33" s="6" t="s">
         <v>19</v>
@@ -1858,12 +1880,12 @@
         <v>84</v>
       </c>
       <c r="E33" s="7" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="34" spans="2:5">
       <c r="B34" s="5" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C34" s="6" t="s">
         <v>19</v>
@@ -1872,7 +1894,7 @@
         <v>84</v>
       </c>
       <c r="E34" s="7" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="35" spans="2:5">
@@ -2084,7 +2106,7 @@
       </c>
       <c r="D52" s="15"/>
       <c r="E52" s="16" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="53" spans="2:5">
@@ -2106,7 +2128,7 @@
       </c>
       <c r="D54" s="6"/>
       <c r="E54" s="7" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="55" spans="2:5">
@@ -2128,7 +2150,7 @@
       </c>
       <c r="D56" s="15"/>
       <c r="E56" s="16" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="57" spans="2:5">
@@ -2150,7 +2172,7 @@
       </c>
       <c r="D58" s="6"/>
       <c r="E58" s="7" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="59" spans="2:5">
@@ -2172,7 +2194,7 @@
       </c>
       <c r="D60" s="12"/>
       <c r="E60" s="13" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="61" spans="2:5">
@@ -2184,7 +2206,7 @@
       </c>
       <c r="D61" s="12"/>
       <c r="E61" s="13" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="62" spans="2:5">
@@ -2196,7 +2218,7 @@
       </c>
       <c r="D62" s="12"/>
       <c r="E62" s="13" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="63" spans="2:5">
@@ -2206,7 +2228,7 @@
       <c r="C63" s="12"/>
       <c r="D63" s="12"/>
       <c r="E63" s="13" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="64" spans="2:5">
@@ -2218,7 +2240,7 @@
       </c>
       <c r="D64" s="12"/>
       <c r="E64" s="13" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="65" spans="2:5">
@@ -2230,7 +2252,7 @@
       </c>
       <c r="D65" s="12"/>
       <c r="E65" s="13" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="66" spans="2:5">
@@ -2242,7 +2264,7 @@
       </c>
       <c r="D66" s="12"/>
       <c r="E66" s="13" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="67" spans="2:5">
@@ -2270,11 +2292,11 @@
         <v>59</v>
       </c>
       <c r="C69" s="15" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D69" s="15"/>
       <c r="E69" s="16" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="70" spans="2:5">
@@ -2282,11 +2304,11 @@
         <v>60</v>
       </c>
       <c r="C70" s="9" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D70" s="9"/>
       <c r="E70" s="10" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="71" spans="2:5">
@@ -2430,7 +2452,7 @@
       </c>
       <c r="D84" s="22"/>
       <c r="E84" s="23" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
   </sheetData>
@@ -2444,7 +2466,7 @@
   <dimension ref="B3:E53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="E35" sqref="E35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2476,10 +2498,10 @@
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="6" spans="2:5">
@@ -2507,7 +2529,7 @@
       </c>
       <c r="D8" s="12"/>
       <c r="E8" s="13" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="9" spans="2:5">
@@ -2519,7 +2541,7 @@
       </c>
       <c r="D9" s="12"/>
       <c r="E9" s="13" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="10" spans="2:5">
@@ -2528,7 +2550,7 @@
       </c>
       <c r="C10" s="12"/>
       <c r="D10" s="12" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E10" s="13"/>
     </row>
@@ -2581,7 +2603,7 @@
       </c>
       <c r="D15" s="12"/>
       <c r="E15" s="13" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="16" spans="2:5">
@@ -2591,7 +2613,7 @@
       <c r="C16" s="12"/>
       <c r="D16" s="12"/>
       <c r="E16" s="13" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="17" spans="2:5">
@@ -2603,7 +2625,7 @@
       </c>
       <c r="D17" s="12"/>
       <c r="E17" s="13" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="18" spans="2:5">
@@ -2615,7 +2637,7 @@
       </c>
       <c r="D18" s="12"/>
       <c r="E18" s="13" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="19" spans="2:5">
@@ -2627,7 +2649,7 @@
       </c>
       <c r="D19" s="12"/>
       <c r="E19" s="13" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="20" spans="2:5">
@@ -2639,7 +2661,7 @@
       </c>
       <c r="D20" s="12"/>
       <c r="E20" s="13" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="21" spans="2:5">
@@ -2651,7 +2673,7 @@
       </c>
       <c r="D21" s="12"/>
       <c r="E21" s="13" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="22" spans="2:5">
@@ -2660,10 +2682,10 @@
       </c>
       <c r="C22" s="12"/>
       <c r="D22" s="12" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="E22" s="13" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="23" spans="2:5">
@@ -2673,7 +2695,7 @@
       <c r="C23" s="12"/>
       <c r="D23" s="12"/>
       <c r="E23" s="13" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="24" spans="2:5">
@@ -2685,7 +2707,7 @@
       </c>
       <c r="D24" s="12"/>
       <c r="E24" s="13" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="25" spans="2:5">
@@ -2697,7 +2719,7 @@
       </c>
       <c r="D25" s="12"/>
       <c r="E25" s="13" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="26" spans="2:5">
@@ -2707,7 +2729,7 @@
       <c r="C26" s="6"/>
       <c r="D26" s="6"/>
       <c r="E26" s="7" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="27" spans="2:5">
@@ -2717,7 +2739,7 @@
       <c r="C27" s="6"/>
       <c r="D27" s="6"/>
       <c r="E27" s="7" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="28" spans="2:5">
@@ -2727,7 +2749,7 @@
       <c r="C28" s="6"/>
       <c r="D28" s="6"/>
       <c r="E28" s="7" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="29" spans="2:5">
@@ -2737,7 +2759,7 @@
       <c r="C29" s="6"/>
       <c r="D29" s="6"/>
       <c r="E29" s="7" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="30" spans="2:5">
@@ -2747,7 +2769,7 @@
       <c r="C30" s="6"/>
       <c r="D30" s="6"/>
       <c r="E30" s="7" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="31" spans="2:5">
@@ -2757,7 +2779,7 @@
       <c r="C31" s="6"/>
       <c r="D31" s="6"/>
       <c r="E31" s="7" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="32" spans="2:5">
@@ -2767,7 +2789,7 @@
       <c r="C32" s="6"/>
       <c r="D32" s="6"/>
       <c r="E32" s="7" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="33" spans="2:5">
@@ -2775,13 +2797,13 @@
         <v>127</v>
       </c>
       <c r="C33" s="6" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D33" s="6" t="s">
+        <v>233</v>
+      </c>
+      <c r="E33" s="7" t="s">
         <v>234</v>
-      </c>
-      <c r="E33" s="7" t="s">
-        <v>235</v>
       </c>
     </row>
     <row r="34" spans="2:5">
@@ -2793,7 +2815,7 @@
       </c>
       <c r="D34" s="12"/>
       <c r="E34" s="13" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="35" spans="2:5">
@@ -2803,7 +2825,7 @@
       <c r="C35" s="12"/>
       <c r="D35" s="12"/>
       <c r="E35" s="13" t="s">
-        <v>149</v>
+        <v>280</v>
       </c>
     </row>
     <row r="36" spans="2:5">
@@ -2815,7 +2837,7 @@
       </c>
       <c r="D36" s="12"/>
       <c r="E36" s="13" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="37" spans="2:5">
@@ -2827,7 +2849,7 @@
       </c>
       <c r="D37" s="12"/>
       <c r="E37" s="13" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="38" spans="2:5">
@@ -2839,7 +2861,7 @@
       </c>
       <c r="D38" s="12"/>
       <c r="E38" s="13" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="39" spans="2:5">
@@ -2851,7 +2873,7 @@
       </c>
       <c r="D39" s="12"/>
       <c r="E39" s="13" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="40" spans="2:5">
@@ -2870,10 +2892,10 @@
       </c>
       <c r="C41" s="12"/>
       <c r="D41" s="12" t="s">
+        <v>239</v>
+      </c>
+      <c r="E41" s="13" t="s">
         <v>240</v>
-      </c>
-      <c r="E41" s="13" t="s">
-        <v>241</v>
       </c>
     </row>
     <row r="42" spans="2:5">
@@ -2883,7 +2905,7 @@
       <c r="C42" s="12"/>
       <c r="D42" s="12"/>
       <c r="E42" s="13" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="43" spans="2:5">
@@ -2894,10 +2916,10 @@
         <v>112</v>
       </c>
       <c r="D43" s="12" t="s">
+        <v>242</v>
+      </c>
+      <c r="E43" s="13" t="s">
         <v>243</v>
-      </c>
-      <c r="E43" s="13" t="s">
-        <v>244</v>
       </c>
     </row>
     <row r="44" spans="2:5">
@@ -2909,7 +2931,7 @@
       </c>
       <c r="D44" s="12"/>
       <c r="E44" s="13" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="45" spans="2:5">
@@ -2941,7 +2963,7 @@
       </c>
       <c r="D47" s="6"/>
       <c r="E47" s="7" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="48" spans="2:5">
@@ -2963,7 +2985,7 @@
       </c>
       <c r="D49" s="6"/>
       <c r="E49" s="7" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="50" spans="2:5">
@@ -2985,7 +3007,7 @@
       </c>
       <c r="D51" s="12"/>
       <c r="E51" s="13" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="52" spans="2:5">
@@ -2995,7 +3017,7 @@
       <c r="C52" s="12"/>
       <c r="D52" s="12"/>
       <c r="E52" s="13" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="53" spans="2:5" ht="15.75" thickBot="1">
@@ -3004,10 +3026,10 @@
       </c>
       <c r="C53" s="22"/>
       <c r="D53" s="22" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="E53" s="23" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
   </sheetData>
@@ -3051,420 +3073,420 @@
     <row r="4" spans="2:5" ht="15.75" thickBot="1"/>
     <row r="5" spans="2:5">
       <c r="B5" s="25" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C5" s="26" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D5" s="26" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E5" s="27" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="6" spans="2:5">
       <c r="B6" s="11" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D6" s="12"/>
       <c r="E6" s="13" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="7" spans="2:5">
       <c r="B7" s="5" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="D7" s="6"/>
       <c r="E7" s="7" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="8" spans="2:5">
       <c r="B8" s="5" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="D8" s="6"/>
       <c r="E8" s="10" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="9" spans="2:5">
       <c r="B9" s="14" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C9" s="15" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D9" s="15"/>
       <c r="E9" s="16"/>
     </row>
     <row r="10" spans="2:5">
       <c r="B10" s="5" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D10" s="6"/>
       <c r="E10" s="7" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="11" spans="2:5">
       <c r="B11" s="5" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D11" s="6"/>
       <c r="E11" s="7"/>
     </row>
     <row r="12" spans="2:5">
       <c r="B12" s="8" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D12" s="9"/>
       <c r="E12" s="10" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="13" spans="2:5">
       <c r="B13" s="5" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="D13" s="6"/>
       <c r="E13" s="7" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="14" spans="2:5">
       <c r="B14" s="5" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="D14" s="6"/>
       <c r="E14" s="7"/>
     </row>
     <row r="15" spans="2:5">
       <c r="B15" s="11" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C15" s="12" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D15" s="12"/>
       <c r="E15" s="13"/>
     </row>
     <row r="16" spans="2:5">
       <c r="B16" s="11" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C16" s="12"/>
       <c r="D16" s="12" t="s">
+        <v>194</v>
+      </c>
+      <c r="E16" s="13" t="s">
         <v>195</v>
-      </c>
-      <c r="E16" s="13" t="s">
-        <v>196</v>
       </c>
     </row>
     <row r="17" spans="2:5">
       <c r="B17" s="5" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D17" s="6"/>
       <c r="E17" s="7"/>
     </row>
     <row r="18" spans="2:5">
       <c r="B18" s="11" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C18" s="12" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D18" s="12"/>
       <c r="E18" s="13" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="19" spans="2:5">
       <c r="B19" s="11" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C19" s="12" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D19" s="12"/>
       <c r="E19" s="13" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="20" spans="2:5">
       <c r="B20" s="14" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C20" s="15"/>
       <c r="D20" s="15" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E20" s="16" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="21" spans="2:5">
       <c r="B21" s="8" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C21" s="9"/>
       <c r="D21" s="9" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E21" s="10" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="22" spans="2:5">
       <c r="B22" s="5" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D22" s="6"/>
       <c r="E22" s="7"/>
     </row>
     <row r="23" spans="2:5">
       <c r="B23" s="5" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D23" s="6"/>
       <c r="E23" s="7"/>
     </row>
     <row r="24" spans="2:5">
       <c r="B24" s="5" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D24" s="6"/>
       <c r="E24" s="7"/>
     </row>
     <row r="25" spans="2:5">
       <c r="B25" s="5" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D25" s="6"/>
       <c r="E25" s="7"/>
     </row>
     <row r="26" spans="2:5">
       <c r="B26" s="5" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D26" s="6"/>
       <c r="E26" s="7"/>
     </row>
     <row r="27" spans="2:5">
       <c r="B27" s="5" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D27" s="6"/>
       <c r="E27" s="7"/>
     </row>
     <row r="28" spans="2:5">
       <c r="B28" s="5" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D28" s="6"/>
       <c r="E28" s="7"/>
     </row>
     <row r="29" spans="2:5">
       <c r="B29" s="5" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C29" s="6" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D29" s="6"/>
       <c r="E29" s="7"/>
     </row>
     <row r="30" spans="2:5">
       <c r="B30" s="5" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D30" s="6"/>
       <c r="E30" s="7"/>
     </row>
     <row r="31" spans="2:5">
       <c r="B31" s="11" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C31" s="12"/>
       <c r="D31" s="12"/>
       <c r="E31" s="13" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="32" spans="2:5">
       <c r="B32" s="14" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C32" s="15" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="D32" s="15"/>
       <c r="E32" s="16" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="33" spans="2:5">
       <c r="B33" s="5" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C33" s="6" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="D33" s="6"/>
       <c r="E33" s="7" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="34" spans="2:5">
       <c r="B34" s="5" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C34" s="6" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="D34" s="6"/>
       <c r="E34" s="7" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="35" spans="2:5">
       <c r="B35" s="5" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C35" s="6" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="D35" s="6"/>
       <c r="E35" s="7" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="36" spans="2:5">
       <c r="B36" s="5" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C36" s="6" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="D36" s="6"/>
       <c r="E36" s="7" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="37" spans="2:5">
       <c r="B37" s="8" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C37" s="9" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="D37" s="9"/>
       <c r="E37" s="10" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="38" spans="2:5">
       <c r="B38" s="5" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C38" s="6" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D38" s="6"/>
       <c r="E38" s="7"/>
     </row>
     <row r="39" spans="2:5">
       <c r="B39" s="5" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C39" s="6" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D39" s="6"/>
       <c r="E39" s="7" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="40" spans="2:5">
       <c r="B40" s="5" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C40" s="6" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D40" s="6"/>
       <c r="E40" s="7"/>
     </row>
     <row r="41" spans="2:5">
       <c r="B41" s="5" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C41" s="6" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D41" s="6"/>
       <c r="E41" s="7"/>
     </row>
     <row r="42" spans="2:5" ht="15.75" thickBot="1">
       <c r="B42" s="17" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C42" s="6" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D42" s="18"/>
       <c r="E42" s="19"/>
@@ -3479,162 +3501,257 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="C2:K12"/>
+  <dimension ref="A1:H18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M6" sqref="M6:M8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="11" max="11" width="9.5703125" style="28" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.7109375" customWidth="1"/>
+    <col min="2" max="2" width="14.42578125" customWidth="1"/>
+    <col min="4" max="5" width="12.7109375" style="29" customWidth="1"/>
+    <col min="6" max="6" width="12.7109375" style="28" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:11">
-      <c r="G2">
+    <row r="1" spans="1:8">
+      <c r="H1" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="D2" s="29">
         <v>25.4</v>
       </c>
-      <c r="I2">
+      <c r="E2" s="29">
         <v>72</v>
       </c>
-      <c r="K2" s="28">
+      <c r="F2" s="28">
         <v>65536</v>
       </c>
     </row>
-    <row r="3" spans="3:11">
-      <c r="E3" t="s">
+    <row r="3" spans="1:8">
+      <c r="A3" t="s">
+        <v>281</v>
+      </c>
+      <c r="C3" t="s">
+        <v>271</v>
+      </c>
+      <c r="D3" s="29" t="s">
+        <v>274</v>
+      </c>
+      <c r="E3" s="29" t="s">
+        <v>275</v>
+      </c>
+      <c r="F3" s="28" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="B4" t="s">
+        <v>270</v>
+      </c>
+      <c r="C4">
+        <v>210</v>
+      </c>
+      <c r="D4" s="29">
+        <f>C4/$D$2</f>
+        <v>8.2677165354330722</v>
+      </c>
+      <c r="E4" s="29">
+        <f>D4*$E$2</f>
+        <v>595.27559055118115</v>
+      </c>
+      <c r="F4" s="28">
+        <f>E4*$F$2</f>
+        <v>39011981.102362208</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="B5" t="s">
+        <v>273</v>
+      </c>
+      <c r="C5">
+        <v>12</v>
+      </c>
+      <c r="D5" s="29">
+        <f>C5/$D$2</f>
+        <v>0.47244094488188981</v>
+      </c>
+      <c r="E5" s="29">
+        <f>D5*$E$2</f>
+        <v>34.015748031496067</v>
+      </c>
+      <c r="F5" s="28">
+        <f>E5*$F$2</f>
+        <v>2229256.0629921262</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="B6" t="s">
         <v>272</v>
       </c>
-      <c r="G3" t="s">
-        <v>275</v>
-      </c>
-      <c r="I3" t="s">
-        <v>276</v>
-      </c>
-      <c r="K3" s="28" t="s">
+      <c r="C6">
+        <f>C4-(2*C5)</f>
+        <v>186</v>
+      </c>
+      <c r="D6" s="29">
+        <f>C6/$D$2</f>
+        <v>7.3228346456692917</v>
+      </c>
+      <c r="E6" s="29">
+        <f>D6*$E$2</f>
+        <v>527.24409448818903</v>
+      </c>
+      <c r="F6" s="28">
+        <f>E6*$F$2</f>
+        <v>34553468.976377957</v>
+      </c>
+      <c r="G6" s="28"/>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="G7" s="28"/>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" t="s">
+        <v>284</v>
+      </c>
+      <c r="G8" s="28"/>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="B9" t="s">
+        <v>282</v>
+      </c>
+      <c r="C9">
+        <v>186</v>
+      </c>
+      <c r="G9" s="28"/>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="G10" s="28"/>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="B12" t="s">
         <v>277</v>
       </c>
-    </row>
-    <row r="4" spans="3:11">
-      <c r="C4" t="s">
-        <v>271</v>
-      </c>
-      <c r="E4">
-        <v>210</v>
-      </c>
-      <c r="G4">
-        <f>E4/$G$2</f>
-        <v>8.2677165354330722</v>
-      </c>
-      <c r="I4">
-        <f>G4*$I$2</f>
-        <v>595.27559055118115</v>
-      </c>
-      <c r="K4" s="28">
-        <f>I4*$K$2</f>
-        <v>39011981.102362208</v>
-      </c>
-    </row>
-    <row r="6" spans="3:11">
-      <c r="C6" t="s">
-        <v>274</v>
-      </c>
-      <c r="E6">
-        <v>12</v>
-      </c>
-      <c r="G6">
-        <f>E6/$G$2</f>
-        <v>0.47244094488188981</v>
-      </c>
-      <c r="I6">
-        <f>G6*$I$2</f>
-        <v>34.015748031496067</v>
-      </c>
-      <c r="K6" s="28">
-        <f>I6*$K$2</f>
-        <v>2229256.0629921262</v>
-      </c>
-    </row>
-    <row r="8" spans="3:11">
-      <c r="C8" t="s">
-        <v>273</v>
-      </c>
-      <c r="E8">
-        <f>E4-(2*E6)</f>
-        <v>186</v>
-      </c>
-      <c r="G8">
-        <f>E8/$G$2</f>
-        <v>7.3228346456692917</v>
-      </c>
-      <c r="I8">
-        <f>G8*$I$2</f>
-        <v>527.24409448818903</v>
-      </c>
-      <c r="K8" s="28">
-        <f>I8*$K$2</f>
-        <v>34553468.976377957</v>
-      </c>
-    </row>
-    <row r="10" spans="3:11">
-      <c r="C10" t="s">
+      <c r="C12">
+        <v>35</v>
+      </c>
+      <c r="D12" s="29">
+        <f t="shared" ref="D12:D14" si="0">C12/$D$2</f>
+        <v>1.3779527559055118</v>
+      </c>
+      <c r="E12" s="29">
+        <f t="shared" ref="E12:E14" si="1">D12*$E$2</f>
+        <v>99.212598425196845</v>
+      </c>
+      <c r="F12" s="28">
+        <f>E12*$F$2</f>
+        <v>6501996.8503937004</v>
+      </c>
+      <c r="G12" s="28"/>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="B13" t="s">
         <v>278</v>
       </c>
-      <c r="E10">
-        <v>35</v>
-      </c>
-      <c r="G10">
-        <f t="shared" ref="G10:G12" si="0">E10/$G$2</f>
-        <v>1.3779527559055118</v>
-      </c>
-      <c r="I10">
-        <f t="shared" ref="I10:I12" si="1">G10*$I$2</f>
-        <v>99.212598425196845</v>
-      </c>
-      <c r="K10" s="28">
-        <f>I10*$K$2</f>
-        <v>6501996.8503937004</v>
-      </c>
-    </row>
-    <row r="11" spans="3:11">
-      <c r="C11" t="s">
-        <v>279</v>
-      </c>
-      <c r="E11">
+      <c r="C13">
         <v>26</v>
       </c>
-      <c r="G11">
+      <c r="D13" s="29">
         <f t="shared" si="0"/>
         <v>1.0236220472440944</v>
       </c>
-      <c r="I11">
+      <c r="E13" s="29">
         <f t="shared" si="1"/>
         <v>73.7007874015748</v>
       </c>
-      <c r="K11" s="28">
-        <f>I11*$K$2</f>
+      <c r="F13" s="28">
+        <f>E13*$F$2</f>
         <v>4830054.8031496061</v>
       </c>
-    </row>
-    <row r="12" spans="3:11">
-      <c r="C12" t="s">
-        <v>280</v>
-      </c>
-      <c r="E12">
-        <f>E8-E10-E11</f>
+      <c r="G13" s="28"/>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="B14" t="s">
+        <v>279</v>
+      </c>
+      <c r="C14">
+        <f>C6-C13-C12</f>
         <v>125</v>
       </c>
-      <c r="G12">
+      <c r="D14" s="29">
         <f t="shared" si="0"/>
         <v>4.9212598425196852</v>
       </c>
-      <c r="I12">
+      <c r="E14" s="29">
         <f t="shared" si="1"/>
         <v>354.33070866141736</v>
       </c>
-      <c r="K12" s="28">
-        <f>I12*$K$2</f>
+      <c r="F14" s="28">
+        <f>E14*$F$2</f>
         <v>23221417.322834648</v>
+      </c>
+      <c r="G14" s="28"/>
+      <c r="H14" s="28">
+        <f>SUM(F12:F14)-F$6</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="A16" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8">
+      <c r="B17" t="s">
+        <v>277</v>
+      </c>
+      <c r="C17">
+        <v>45</v>
+      </c>
+      <c r="D17" s="29">
+        <f t="shared" ref="D17:D18" si="2">C17/$D$2</f>
+        <v>1.7716535433070868</v>
+      </c>
+      <c r="E17" s="29">
+        <f t="shared" ref="E17:E18" si="3">D17*$E$2</f>
+        <v>127.55905511811025</v>
+      </c>
+      <c r="F17" s="28">
+        <f t="shared" ref="F17:F18" si="4">E17*$F$2</f>
+        <v>8359710.2362204734</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8">
+      <c r="B18" t="s">
+        <v>278</v>
+      </c>
+      <c r="C18">
+        <f>C6-C17</f>
+        <v>141</v>
+      </c>
+      <c r="D18" s="29">
+        <f t="shared" si="2"/>
+        <v>5.5511811023622046</v>
+      </c>
+      <c r="E18" s="29">
+        <f t="shared" si="3"/>
+        <v>399.68503937007875</v>
+      </c>
+      <c r="F18" s="28">
+        <f>E18*$F$2</f>
+        <v>26193758.740157481</v>
+      </c>
+      <c r="H18" s="28">
+        <f>SUM(F16:F18)-F$6</f>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
More changes to the mappings and the proto template for the format changes
</commit_message>
<xml_diff>
--- a/readme/XJDF Format Mappings.xlsx
+++ b/readme/XJDF Format Mappings.xlsx
@@ -265,9 +265,6 @@
     <t>Comments/Usage</t>
   </si>
   <si>
-    <t xml:space="preserve">Chapter title heading for the Appendices </t>
-  </si>
-  <si>
     <t>Manual Action Rqd</t>
   </si>
   <si>
@@ -878,6 +875,9 @@
   </si>
   <si>
     <t>Check!</t>
+  </si>
+  <si>
+    <t>Chapter title heading for the Appendices  Now the same as Chapters - its there is a special Master Page</t>
   </si>
 </sst>
 </file>
@@ -885,7 +885,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="0.00000"/>
+    <numFmt numFmtId="164" formatCode="0.00000"/>
   </numFmts>
   <fonts count="2">
     <font>
@@ -1207,7 +1207,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1507,8 +1507,8 @@
   </sheetPr>
   <dimension ref="B3:E84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="B64" sqref="B64"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9:C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1528,7 +1528,7 @@
         <v>79</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>81</v>
@@ -1556,7 +1556,7 @@
       </c>
       <c r="D6" s="6"/>
       <c r="E6" s="7" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="7" spans="2:5">
@@ -1584,11 +1584,11 @@
         <v>4</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>4</v>
+        <v>30</v>
       </c>
       <c r="D9" s="12"/>
       <c r="E9" s="13" t="s">
-        <v>82</v>
+        <v>286</v>
       </c>
     </row>
     <row r="10" spans="2:5">
@@ -1642,7 +1642,7 @@
       </c>
       <c r="D14" s="9"/>
       <c r="E14" s="10" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="15" spans="2:5">
@@ -1654,7 +1654,7 @@
       </c>
       <c r="D15" s="12"/>
       <c r="E15" s="13" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="16" spans="2:5">
@@ -1666,7 +1666,7 @@
       </c>
       <c r="D16" s="12"/>
       <c r="E16" s="13" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="17" spans="2:5">
@@ -1678,7 +1678,7 @@
       </c>
       <c r="D17" s="12"/>
       <c r="E17" s="13" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="18" spans="2:5">
@@ -1689,7 +1689,7 @@
         <v>13</v>
       </c>
       <c r="D18" s="15" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E18" s="16"/>
     </row>
@@ -1701,7 +1701,7 @@
         <v>14</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E19" s="7"/>
     </row>
@@ -1713,7 +1713,7 @@
         <v>15</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E20" s="7"/>
     </row>
@@ -1725,7 +1725,7 @@
         <v>16</v>
       </c>
       <c r="D21" s="9" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E21" s="7"/>
     </row>
@@ -1738,7 +1738,7 @@
       </c>
       <c r="D22" s="15"/>
       <c r="E22" s="16" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="23" spans="2:5">
@@ -1750,7 +1750,7 @@
       </c>
       <c r="D23" s="9"/>
       <c r="E23" s="10" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="24" spans="2:5">
@@ -1762,7 +1762,7 @@
       </c>
       <c r="D24" s="6"/>
       <c r="E24" s="7" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="25" spans="2:5">
@@ -1773,7 +1773,7 @@
         <v>19</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E25" s="7"/>
     </row>
@@ -1785,7 +1785,7 @@
         <v>19</v>
       </c>
       <c r="D26" s="6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E26" s="7"/>
     </row>
@@ -1797,7 +1797,7 @@
         <v>19</v>
       </c>
       <c r="D27" s="6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E27" s="7"/>
     </row>
@@ -1809,52 +1809,52 @@
         <v>19</v>
       </c>
       <c r="D28" s="20" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E28" s="7" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="29" spans="2:5">
       <c r="B29" s="5" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C29" s="6" t="s">
         <v>19</v>
       </c>
       <c r="D29" s="6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E29" s="7" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="30" spans="2:5">
       <c r="B30" s="5" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C30" s="6" t="s">
         <v>19</v>
       </c>
       <c r="D30" s="6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E30" s="7" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="31" spans="2:5">
       <c r="B31" s="5" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C31" s="6" t="s">
         <v>19</v>
       </c>
       <c r="D31" s="6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E31" s="7" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="32" spans="2:5">
@@ -1865,36 +1865,36 @@
         <v>19</v>
       </c>
       <c r="D32" s="6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E32" s="7"/>
     </row>
     <row r="33" spans="2:5">
       <c r="B33" s="5" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C33" s="6" t="s">
         <v>19</v>
       </c>
       <c r="D33" s="6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E33" s="7" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="34" spans="2:5">
       <c r="B34" s="5" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C34" s="6" t="s">
         <v>19</v>
       </c>
       <c r="D34" s="6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E34" s="7" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="35" spans="2:5">
@@ -1905,7 +1905,7 @@
         <v>19</v>
       </c>
       <c r="D35" s="6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E35" s="7"/>
     </row>
@@ -1917,7 +1917,7 @@
         <v>19</v>
       </c>
       <c r="D36" s="6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E36" s="7"/>
     </row>
@@ -1930,7 +1930,7 @@
       </c>
       <c r="D37" s="12"/>
       <c r="E37" s="13" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="38" spans="2:5">
@@ -1942,7 +1942,7 @@
       </c>
       <c r="D38" s="12"/>
       <c r="E38" s="13" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="39" spans="2:5">
@@ -1954,7 +1954,7 @@
       </c>
       <c r="D39" s="12"/>
       <c r="E39" s="13" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="40" spans="2:5">
@@ -1966,7 +1966,7 @@
       </c>
       <c r="D40" s="12"/>
       <c r="E40" s="13" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="41" spans="2:5">
@@ -1974,13 +1974,13 @@
         <v>31</v>
       </c>
       <c r="C41" s="15" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D41" s="15" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E41" s="16" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="42" spans="2:5">
@@ -1988,11 +1988,11 @@
         <v>32</v>
       </c>
       <c r="C42" s="6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D42" s="6"/>
       <c r="E42" s="7" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="43" spans="2:5">
@@ -2000,11 +2000,11 @@
         <v>33</v>
       </c>
       <c r="C43" s="6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D43" s="6"/>
       <c r="E43" s="7" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="44" spans="2:5">
@@ -2012,11 +2012,11 @@
         <v>34</v>
       </c>
       <c r="C44" s="6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D44" s="6"/>
       <c r="E44" s="7" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="45" spans="2:5">
@@ -2024,11 +2024,11 @@
         <v>35</v>
       </c>
       <c r="C45" s="9" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D45" s="9"/>
       <c r="E45" s="10" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="46" spans="2:5">
@@ -2040,7 +2040,7 @@
       </c>
       <c r="D46" s="12"/>
       <c r="E46" s="13" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="47" spans="2:5">
@@ -2052,7 +2052,7 @@
       </c>
       <c r="D47" s="9"/>
       <c r="E47" s="10" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="48" spans="2:5">
@@ -2091,10 +2091,10 @@
       </c>
       <c r="C51" s="12"/>
       <c r="D51" s="12" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E51" s="13" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="52" spans="2:5">
@@ -2106,7 +2106,7 @@
       </c>
       <c r="D52" s="15"/>
       <c r="E52" s="16" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="53" spans="2:5">
@@ -2128,7 +2128,7 @@
       </c>
       <c r="D54" s="6"/>
       <c r="E54" s="7" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="55" spans="2:5">
@@ -2150,7 +2150,7 @@
       </c>
       <c r="D56" s="15"/>
       <c r="E56" s="16" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="57" spans="2:5">
@@ -2172,7 +2172,7 @@
       </c>
       <c r="D58" s="6"/>
       <c r="E58" s="7" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="59" spans="2:5">
@@ -2194,7 +2194,7 @@
       </c>
       <c r="D60" s="12"/>
       <c r="E60" s="13" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="61" spans="2:5">
@@ -2206,7 +2206,7 @@
       </c>
       <c r="D61" s="12"/>
       <c r="E61" s="13" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="62" spans="2:5">
@@ -2218,7 +2218,7 @@
       </c>
       <c r="D62" s="12"/>
       <c r="E62" s="13" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="63" spans="2:5">
@@ -2228,7 +2228,7 @@
       <c r="C63" s="12"/>
       <c r="D63" s="12"/>
       <c r="E63" s="13" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="64" spans="2:5">
@@ -2240,7 +2240,7 @@
       </c>
       <c r="D64" s="12"/>
       <c r="E64" s="13" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="65" spans="2:5">
@@ -2252,7 +2252,7 @@
       </c>
       <c r="D65" s="12"/>
       <c r="E65" s="13" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="66" spans="2:5">
@@ -2264,7 +2264,7 @@
       </c>
       <c r="D66" s="12"/>
       <c r="E66" s="13" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="67" spans="2:5">
@@ -2292,11 +2292,11 @@
         <v>59</v>
       </c>
       <c r="C69" s="15" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D69" s="15"/>
       <c r="E69" s="16" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="70" spans="2:5">
@@ -2304,11 +2304,11 @@
         <v>60</v>
       </c>
       <c r="C70" s="9" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D70" s="9"/>
       <c r="E70" s="10" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="71" spans="2:5">
@@ -2452,7 +2452,7 @@
       </c>
       <c r="D84" s="22"/>
       <c r="E84" s="23" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
   </sheetData>
@@ -2485,7 +2485,7 @@
         <v>79</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>81</v>
@@ -2494,19 +2494,19 @@
     <row r="4" spans="2:5" ht="15.75" thickBot="1"/>
     <row r="5" spans="2:5">
       <c r="B5" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="3" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="6" spans="2:5">
       <c r="B6" s="5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C6" s="6"/>
       <c r="D6" s="6"/>
@@ -2514,7 +2514,7 @@
     </row>
     <row r="7" spans="2:5">
       <c r="B7" s="5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C7" s="6"/>
       <c r="D7" s="6"/>
@@ -2522,514 +2522,514 @@
     </row>
     <row r="8" spans="2:5">
       <c r="B8" s="11" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D8" s="12"/>
       <c r="E8" s="13" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="9" spans="2:5">
       <c r="B9" s="11" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D9" s="12"/>
       <c r="E9" s="13" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="10" spans="2:5">
       <c r="B10" s="11" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C10" s="12"/>
       <c r="D10" s="12" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E10" s="13"/>
     </row>
     <row r="11" spans="2:5">
       <c r="B11" s="11" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D11" s="12"/>
       <c r="E11" s="13"/>
     </row>
     <row r="12" spans="2:5">
       <c r="B12" s="11" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D12" s="12"/>
       <c r="E12" s="13"/>
     </row>
     <row r="13" spans="2:5">
       <c r="B13" s="11" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D13" s="12"/>
       <c r="E13" s="13"/>
     </row>
     <row r="14" spans="2:5">
       <c r="B14" s="11" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D14" s="12"/>
       <c r="E14" s="13"/>
     </row>
     <row r="15" spans="2:5">
       <c r="B15" s="11" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C15" s="24" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D15" s="12"/>
       <c r="E15" s="13" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="16" spans="2:5">
       <c r="B16" s="11" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C16" s="12"/>
       <c r="D16" s="12"/>
       <c r="E16" s="13" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="17" spans="2:5">
       <c r="B17" s="11" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C17" s="12" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D17" s="12"/>
       <c r="E17" s="13" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="18" spans="2:5">
       <c r="B18" s="11" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C18" s="12" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D18" s="12"/>
       <c r="E18" s="13" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="19" spans="2:5">
       <c r="B19" s="11" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C19" s="12" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D19" s="12"/>
       <c r="E19" s="13" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="20" spans="2:5">
       <c r="B20" s="11" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C20" s="12" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D20" s="12"/>
       <c r="E20" s="13" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="21" spans="2:5">
       <c r="B21" s="11" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C21" s="12" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D21" s="12"/>
       <c r="E21" s="13" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="22" spans="2:5">
       <c r="B22" s="11" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C22" s="12"/>
       <c r="D22" s="12" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="E22" s="13" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="23" spans="2:5">
       <c r="B23" s="11" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C23" s="12"/>
       <c r="D23" s="12"/>
       <c r="E23" s="13" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="24" spans="2:5">
       <c r="B24" s="11" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C24" s="12" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D24" s="12"/>
       <c r="E24" s="13" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="25" spans="2:5">
       <c r="B25" s="11" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C25" s="12" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D25" s="12"/>
       <c r="E25" s="13" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="26" spans="2:5">
       <c r="B26" s="5" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C26" s="6"/>
       <c r="D26" s="6"/>
       <c r="E26" s="7" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="27" spans="2:5">
       <c r="B27" s="5" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C27" s="6"/>
       <c r="D27" s="6"/>
       <c r="E27" s="7" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="28" spans="2:5">
       <c r="B28" s="5" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C28" s="6"/>
       <c r="D28" s="6"/>
       <c r="E28" s="7" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="29" spans="2:5">
       <c r="B29" s="5" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C29" s="6"/>
       <c r="D29" s="6"/>
       <c r="E29" s="7" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="30" spans="2:5">
       <c r="B30" s="5" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C30" s="6"/>
       <c r="D30" s="6"/>
       <c r="E30" s="7" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="31" spans="2:5">
       <c r="B31" s="5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C31" s="6"/>
       <c r="D31" s="6"/>
       <c r="E31" s="7" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="32" spans="2:5">
       <c r="B32" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C32" s="6"/>
       <c r="D32" s="6"/>
       <c r="E32" s="7" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="33" spans="2:5">
       <c r="B33" s="5" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C33" s="6" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D33" s="6" t="s">
+        <v>232</v>
+      </c>
+      <c r="E33" s="7" t="s">
         <v>233</v>
-      </c>
-      <c r="E33" s="7" t="s">
-        <v>234</v>
       </c>
     </row>
     <row r="34" spans="2:5">
       <c r="B34" s="11" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C34" s="12" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D34" s="12"/>
       <c r="E34" s="13" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="35" spans="2:5">
       <c r="B35" s="11" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C35" s="12"/>
       <c r="D35" s="12"/>
       <c r="E35" s="13" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="36" spans="2:5">
       <c r="B36" s="11" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C36" s="12" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D36" s="12"/>
       <c r="E36" s="13" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="37" spans="2:5">
       <c r="B37" s="11" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C37" s="12" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D37" s="12"/>
       <c r="E37" s="13" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="38" spans="2:5">
       <c r="B38" s="11" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C38" s="12" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D38" s="12"/>
       <c r="E38" s="13" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="39" spans="2:5">
       <c r="B39" s="11" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C39" s="12" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D39" s="12"/>
       <c r="E39" s="13" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="40" spans="2:5">
       <c r="B40" s="11" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C40" s="12" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D40" s="12"/>
       <c r="E40" s="13"/>
     </row>
     <row r="41" spans="2:5">
       <c r="B41" s="11" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C41" s="12"/>
       <c r="D41" s="12" t="s">
+        <v>238</v>
+      </c>
+      <c r="E41" s="13" t="s">
         <v>239</v>
-      </c>
-      <c r="E41" s="13" t="s">
-        <v>240</v>
       </c>
     </row>
     <row r="42" spans="2:5">
       <c r="B42" s="11" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C42" s="12"/>
       <c r="D42" s="12"/>
       <c r="E42" s="13" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="43" spans="2:5">
       <c r="B43" s="11" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C43" s="12" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D43" s="12" t="s">
+        <v>241</v>
+      </c>
+      <c r="E43" s="13" t="s">
         <v>242</v>
-      </c>
-      <c r="E43" s="13" t="s">
-        <v>243</v>
       </c>
     </row>
     <row r="44" spans="2:5">
       <c r="B44" s="11" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C44" s="12" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D44" s="12"/>
       <c r="E44" s="13" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="45" spans="2:5">
       <c r="B45" s="5" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C45" s="6" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D45" s="6"/>
       <c r="E45" s="7"/>
     </row>
     <row r="46" spans="2:5">
       <c r="B46" s="5" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C46" s="6" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D46" s="6"/>
       <c r="E46" s="7"/>
     </row>
     <row r="47" spans="2:5">
       <c r="B47" s="5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C47" s="6" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D47" s="6"/>
       <c r="E47" s="7" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="48" spans="2:5">
       <c r="B48" s="5" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C48" s="6" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D48" s="6"/>
       <c r="E48" s="7"/>
     </row>
     <row r="49" spans="2:5">
       <c r="B49" s="5" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C49" s="6" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D49" s="6"/>
       <c r="E49" s="7" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="50" spans="2:5">
       <c r="B50" s="5" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C50" s="6" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D50" s="6"/>
       <c r="E50" s="7"/>
     </row>
     <row r="51" spans="2:5">
       <c r="B51" s="11" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C51" s="6" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D51" s="12"/>
       <c r="E51" s="13" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="52" spans="2:5">
       <c r="B52" s="11" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C52" s="12"/>
       <c r="D52" s="12"/>
       <c r="E52" s="13" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="53" spans="2:5" ht="15.75" thickBot="1">
       <c r="B53" s="21" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C53" s="22"/>
       <c r="D53" s="22" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="E53" s="23" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
   </sheetData>
@@ -3064,7 +3064,7 @@
         <v>79</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>81</v>
@@ -3073,420 +3073,420 @@
     <row r="4" spans="2:5" ht="15.75" thickBot="1"/>
     <row r="5" spans="2:5">
       <c r="B5" s="25" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C5" s="26" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D5" s="26" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E5" s="27" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="6" spans="2:5">
       <c r="B6" s="11" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="D6" s="12"/>
       <c r="E6" s="13" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="7" spans="2:5">
       <c r="B7" s="5" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D7" s="6"/>
       <c r="E7" s="7" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="8" spans="2:5">
       <c r="B8" s="5" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D8" s="6"/>
       <c r="E8" s="10" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="9" spans="2:5">
       <c r="B9" s="14" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C9" s="15" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="D9" s="15"/>
       <c r="E9" s="16"/>
     </row>
     <row r="10" spans="2:5">
       <c r="B10" s="5" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="D10" s="6"/>
       <c r="E10" s="7" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="11" spans="2:5">
       <c r="B11" s="5" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="D11" s="6"/>
       <c r="E11" s="7"/>
     </row>
     <row r="12" spans="2:5">
       <c r="B12" s="8" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="D12" s="9"/>
       <c r="E12" s="10" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="13" spans="2:5">
       <c r="B13" s="5" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D13" s="6"/>
       <c r="E13" s="7" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="14" spans="2:5">
       <c r="B14" s="5" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D14" s="6"/>
       <c r="E14" s="7"/>
     </row>
     <row r="15" spans="2:5">
       <c r="B15" s="11" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C15" s="12" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D15" s="12"/>
       <c r="E15" s="13"/>
     </row>
     <row r="16" spans="2:5">
       <c r="B16" s="11" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C16" s="12"/>
       <c r="D16" s="12" t="s">
+        <v>193</v>
+      </c>
+      <c r="E16" s="13" t="s">
         <v>194</v>
-      </c>
-      <c r="E16" s="13" t="s">
-        <v>195</v>
       </c>
     </row>
     <row r="17" spans="2:5">
       <c r="B17" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D17" s="6"/>
       <c r="E17" s="7"/>
     </row>
     <row r="18" spans="2:5">
       <c r="B18" s="11" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C18" s="12" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D18" s="12"/>
       <c r="E18" s="13" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="19" spans="2:5">
       <c r="B19" s="11" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C19" s="12" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D19" s="12"/>
       <c r="E19" s="13" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="20" spans="2:5">
       <c r="B20" s="14" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C20" s="15"/>
       <c r="D20" s="15" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E20" s="16" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="21" spans="2:5">
       <c r="B21" s="8" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C21" s="9"/>
       <c r="D21" s="9" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E21" s="10" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="22" spans="2:5">
       <c r="B22" s="5" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D22" s="6"/>
       <c r="E22" s="7"/>
     </row>
     <row r="23" spans="2:5">
       <c r="B23" s="5" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D23" s="6"/>
       <c r="E23" s="7"/>
     </row>
     <row r="24" spans="2:5">
       <c r="B24" s="5" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D24" s="6"/>
       <c r="E24" s="7"/>
     </row>
     <row r="25" spans="2:5">
       <c r="B25" s="5" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D25" s="6"/>
       <c r="E25" s="7"/>
     </row>
     <row r="26" spans="2:5">
       <c r="B26" s="5" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D26" s="6"/>
       <c r="E26" s="7"/>
     </row>
     <row r="27" spans="2:5">
       <c r="B27" s="5" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D27" s="6"/>
       <c r="E27" s="7"/>
     </row>
     <row r="28" spans="2:5">
       <c r="B28" s="5" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D28" s="6"/>
       <c r="E28" s="7"/>
     </row>
     <row r="29" spans="2:5">
       <c r="B29" s="5" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C29" s="6" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D29" s="6"/>
       <c r="E29" s="7"/>
     </row>
     <row r="30" spans="2:5">
       <c r="B30" s="5" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D30" s="6"/>
       <c r="E30" s="7"/>
     </row>
     <row r="31" spans="2:5">
       <c r="B31" s="11" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C31" s="12"/>
       <c r="D31" s="12"/>
       <c r="E31" s="13" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="32" spans="2:5">
       <c r="B32" s="14" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C32" s="15" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="D32" s="15"/>
       <c r="E32" s="16" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="33" spans="2:5">
       <c r="B33" s="5" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C33" s="6" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="D33" s="6"/>
       <c r="E33" s="7" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="34" spans="2:5">
       <c r="B34" s="5" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C34" s="6" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="D34" s="6"/>
       <c r="E34" s="7" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="35" spans="2:5">
       <c r="B35" s="5" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C35" s="6" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="D35" s="6"/>
       <c r="E35" s="7" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="36" spans="2:5">
       <c r="B36" s="5" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C36" s="6" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="D36" s="6"/>
       <c r="E36" s="7" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="37" spans="2:5">
       <c r="B37" s="8" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C37" s="9" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="D37" s="9"/>
       <c r="E37" s="10" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="38" spans="2:5">
       <c r="B38" s="5" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C38" s="6" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D38" s="6"/>
       <c r="E38" s="7"/>
     </row>
     <row r="39" spans="2:5">
       <c r="B39" s="5" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C39" s="6" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D39" s="6"/>
       <c r="E39" s="7" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="40" spans="2:5">
       <c r="B40" s="5" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C40" s="6" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D40" s="6"/>
       <c r="E40" s="7"/>
     </row>
     <row r="41" spans="2:5">
       <c r="B41" s="5" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C41" s="6" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D41" s="6"/>
       <c r="E41" s="7"/>
     </row>
     <row r="42" spans="2:5" ht="15.75" thickBot="1">
       <c r="B42" s="17" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C42" s="6" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D42" s="18"/>
       <c r="E42" s="19"/>
@@ -3517,7 +3517,7 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="H1" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="2" spans="1:8">
@@ -3533,24 +3533,24 @@
     </row>
     <row r="3" spans="1:8">
       <c r="A3" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="C3" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="D3" s="29" t="s">
+        <v>273</v>
+      </c>
+      <c r="E3" s="29" t="s">
         <v>274</v>
       </c>
-      <c r="E3" s="29" t="s">
+      <c r="F3" s="28" t="s">
         <v>275</v>
-      </c>
-      <c r="F3" s="28" t="s">
-        <v>276</v>
       </c>
     </row>
     <row r="4" spans="1:8">
       <c r="B4" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C4">
         <v>210</v>
@@ -3570,7 +3570,7 @@
     </row>
     <row r="5" spans="1:8">
       <c r="B5" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C5">
         <v>12</v>
@@ -3590,7 +3590,7 @@
     </row>
     <row r="6" spans="1:8">
       <c r="B6" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C6">
         <f>C4-(2*C5)</f>
@@ -3615,13 +3615,13 @@
     </row>
     <row r="8" spans="1:8">
       <c r="A8" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="G8" s="28"/>
     </row>
     <row r="9" spans="1:8">
       <c r="B9" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="C9">
         <v>186</v>
@@ -3633,12 +3633,12 @@
     </row>
     <row r="11" spans="1:8">
       <c r="A11" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="12" spans="1:8">
       <c r="B12" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C12">
         <v>35</v>
@@ -3659,7 +3659,7 @@
     </row>
     <row r="13" spans="1:8">
       <c r="B13" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C13">
         <v>26</v>
@@ -3680,7 +3680,7 @@
     </row>
     <row r="14" spans="1:8">
       <c r="B14" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C14">
         <f>C6-C13-C12</f>
@@ -3706,12 +3706,12 @@
     </row>
     <row r="16" spans="1:8">
       <c r="A16" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="17" spans="2:8">
       <c r="B17" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C17">
         <v>45</v>
@@ -3725,13 +3725,13 @@
         <v>127.55905511811025</v>
       </c>
       <c r="F17" s="28">
-        <f t="shared" ref="F17:F18" si="4">E17*$F$2</f>
+        <f t="shared" ref="F17" si="4">E17*$F$2</f>
         <v>8359710.2362204734</v>
       </c>
     </row>
     <row r="18" spans="2:8">
       <c r="B18" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C18">
         <f>C6-C17</f>

</xml_diff>

<commit_message>
Update to how XRefs will be mapped
</commit_message>
<xml_diff>
--- a/readme/XJDF Format Mappings.xlsx
+++ b/readme/XJDF Format Mappings.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-4800" yWindow="1170" windowWidth="24915" windowHeight="14130"/>
+    <workbookView xWindow="-4800" yWindow="1170" windowWidth="24915" windowHeight="14130" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Paragraph" sheetId="1" r:id="rId1"/>
@@ -1507,7 +1507,7 @@
   </sheetPr>
   <dimension ref="B3:E84"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A37" workbookViewId="0">
       <selection activeCell="B9" sqref="B9:C9"/>
     </sheetView>
   </sheetViews>
@@ -3045,8 +3045,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B3:E42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3292,7 +3292,7 @@
         <v>174</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D24" s="6"/>
       <c r="E24" s="7"/>
@@ -3302,7 +3302,7 @@
         <v>164</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>164</v>
+        <v>173</v>
       </c>
       <c r="D25" s="6"/>
       <c r="E25" s="7"/>

</xml_diff>

<commit_message>
More on cross reference changes
</commit_message>
<xml_diff>
--- a/readme/XJDF Format Mappings.xlsx
+++ b/readme/XJDF Format Mappings.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="469" uniqueCount="287">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="471" uniqueCount="287">
   <si>
     <t>AnchorFigure</t>
   </si>
@@ -3046,7 +3046,7 @@
   <dimension ref="B3:E42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3201,7 +3201,9 @@
       <c r="B16" s="11" t="s">
         <v>169</v>
       </c>
-      <c r="C16" s="12"/>
+      <c r="C16" s="6" t="s">
+        <v>170</v>
+      </c>
       <c r="D16" s="12" t="s">
         <v>193</v>
       </c>
@@ -3295,7 +3297,9 @@
         <v>173</v>
       </c>
       <c r="D24" s="6"/>
-      <c r="E24" s="7"/>
+      <c r="E24" s="7" t="s">
+        <v>150</v>
+      </c>
     </row>
     <row r="25" spans="2:5">
       <c r="B25" s="5" t="s">
@@ -3312,7 +3316,7 @@
         <v>185</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>185</v>
+        <v>170</v>
       </c>
       <c r="D26" s="6"/>
       <c r="E26" s="7"/>

</xml_diff>

<commit_message>
More cross reference formats added and purged. Conditioal text flags revised.
</commit_message>
<xml_diff>
--- a/readme/XJDF Format Mappings.xlsx
+++ b/readme/XJDF Format Mappings.xlsx
@@ -4,20 +4,21 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-4800" yWindow="1170" windowWidth="24915" windowHeight="14130" activeTab="2"/>
+    <workbookView xWindow="-15" yWindow="-15" windowWidth="19215" windowHeight="18180"/>
   </bookViews>
   <sheets>
     <sheet name="Paragraph" sheetId="1" r:id="rId1"/>
     <sheet name="Character" sheetId="2" r:id="rId2"/>
     <sheet name="Cross Ref" sheetId="3" r:id="rId3"/>
-    <sheet name="Table widths" sheetId="4" r:id="rId4"/>
+    <sheet name="Conditional Text" sheetId="5" r:id="rId4"/>
+    <sheet name="Table widths" sheetId="6" r:id="rId5"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="471" uniqueCount="287">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="522" uniqueCount="310">
   <si>
     <t>AnchorFigure</t>
   </si>
@@ -265,6 +266,9 @@
     <t>Comments/Usage</t>
   </si>
   <si>
+    <t xml:space="preserve">Chapter title heading for the Appendices </t>
+  </si>
+  <si>
     <t>Manual Action Rqd</t>
   </si>
   <si>
@@ -463,6 +467,9 @@
     <t>Emphasis</t>
   </si>
   <si>
+    <t>Was used to prevent spelling.</t>
+  </si>
+  <si>
     <t>Confirm removal Ok</t>
   </si>
   <si>
@@ -826,58 +833,121 @@
     <t>All become "Example X.Y ShowingOff"</t>
   </si>
   <si>
+    <t>Not Used</t>
+  </si>
+  <si>
+    <t>Delete</t>
+  </si>
+  <si>
+    <t>Figure Number and Title</t>
+  </si>
+  <si>
+    <t>Three cases replaced manually as appropriate</t>
+  </si>
+  <si>
+    <t>Replaced by XJDF in Emphasis character fmt</t>
+  </si>
+  <si>
+    <t>Footnote Number &amp; Page</t>
+  </si>
+  <si>
+    <t>Weird reference to a footnote after a table - not in template, special for Resources/Subelements</t>
+  </si>
+  <si>
+    <t>CaptionWContinued</t>
+  </si>
+  <si>
+    <t>CaptionWSheet</t>
+  </si>
+  <si>
+    <t>Changed</t>
+  </si>
+  <si>
+    <t>Comment</t>
+  </si>
+  <si>
+    <t>Comment-1x</t>
+  </si>
+  <si>
+    <t>Comment-2x</t>
+  </si>
+  <si>
+    <t>Hidden</t>
+  </si>
+  <si>
+    <t>JDF-1x</t>
+  </si>
+  <si>
+    <t>JDF-1x-background</t>
+  </si>
+  <si>
+    <t>JDF-2x</t>
+  </si>
+  <si>
+    <t>JDF-2x-background</t>
+  </si>
+  <si>
+    <t>JDF-neither</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Used by FM </t>
+  </si>
+  <si>
+    <t>Deleted</t>
+  </si>
+  <si>
+    <t>Although not used - I've retained this in case needed by the editors</t>
+  </si>
+  <si>
+    <t>CIP4 standard conditional</t>
+  </si>
+  <si>
+    <t>Column 2</t>
+  </si>
+  <si>
+    <t>Column 1</t>
+  </si>
+  <si>
+    <t>Processes (I/O Resource Tables are two columns)</t>
+  </si>
+  <si>
+    <t>Column 3</t>
+  </si>
+  <si>
+    <t>JMF, Resources, Subelements</t>
+  </si>
+  <si>
+    <t>Column1</t>
+  </si>
+  <si>
+    <t>All Tables that are one column wide get the full flow width - regardless of the document (JMF, Resources, Appx etc)</t>
+  </si>
+  <si>
+    <t>Flow Width</t>
+  </si>
+  <si>
+    <t>Margins</t>
+  </si>
+  <si>
     <t>Page Width</t>
   </si>
   <si>
+    <t>FM Value</t>
+  </si>
+  <si>
+    <t>Points</t>
+  </si>
+  <si>
+    <t>Inches</t>
+  </si>
+  <si>
     <t>mm</t>
   </si>
   <si>
-    <t>Flow Width</t>
-  </si>
-  <si>
-    <t>Margins</t>
-  </si>
-  <si>
-    <t>Inches</t>
-  </si>
-  <si>
-    <t>Points</t>
-  </si>
-  <si>
-    <t>FM Value</t>
-  </si>
-  <si>
-    <t>Column 1</t>
-  </si>
-  <si>
-    <t>Column 2</t>
-  </si>
-  <si>
-    <t>Column 3</t>
-  </si>
-  <si>
-    <t>Was used to prevent spelling - mostly on attribute/element cardinality symbols.</t>
-  </si>
-  <si>
     <t>General page layout</t>
   </si>
   <si>
-    <t>Column1</t>
-  </si>
-  <si>
-    <t>JMF, Resources, Subelements</t>
-  </si>
-  <si>
-    <t>All Tables that are one column wide get the full flow width - regardless of the document (JMF, Resources, Appx etc)</t>
-  </si>
-  <si>
-    <t>Processes (I/O Resource Tables are two columns)</t>
-  </si>
-  <si>
     <t>Check!</t>
-  </si>
-  <si>
-    <t>Chapter title heading for the Appendices  Now the same as Chapters - its there is a special Master Page</t>
   </si>
 </sst>
 </file>
@@ -1507,8 +1577,8 @@
   </sheetPr>
   <dimension ref="B3:E84"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9:C9"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="C65" sqref="C65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1528,7 +1598,7 @@
         <v>79</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>81</v>
@@ -1556,7 +1626,7 @@
       </c>
       <c r="D6" s="6"/>
       <c r="E6" s="7" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
     </row>
     <row r="7" spans="2:5">
@@ -1584,11 +1654,11 @@
         <v>4</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>30</v>
+        <v>4</v>
       </c>
       <c r="D9" s="12"/>
       <c r="E9" s="13" t="s">
-        <v>286</v>
+        <v>82</v>
       </c>
     </row>
     <row r="10" spans="2:5">
@@ -1642,7 +1712,7 @@
       </c>
       <c r="D14" s="9"/>
       <c r="E14" s="10" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
     </row>
     <row r="15" spans="2:5">
@@ -1654,7 +1724,7 @@
       </c>
       <c r="D15" s="12"/>
       <c r="E15" s="13" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
     </row>
     <row r="16" spans="2:5">
@@ -1666,7 +1736,7 @@
       </c>
       <c r="D16" s="12"/>
       <c r="E16" s="13" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
     </row>
     <row r="17" spans="2:5">
@@ -1678,7 +1748,7 @@
       </c>
       <c r="D17" s="12"/>
       <c r="E17" s="13" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
     </row>
     <row r="18" spans="2:5">
@@ -1689,7 +1759,7 @@
         <v>13</v>
       </c>
       <c r="D18" s="15" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="E18" s="16"/>
     </row>
@@ -1701,7 +1771,7 @@
         <v>14</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="E19" s="7"/>
     </row>
@@ -1713,7 +1783,7 @@
         <v>15</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="E20" s="7"/>
     </row>
@@ -1725,7 +1795,7 @@
         <v>16</v>
       </c>
       <c r="D21" s="9" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="E21" s="7"/>
     </row>
@@ -1738,7 +1808,7 @@
       </c>
       <c r="D22" s="15"/>
       <c r="E22" s="16" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
     </row>
     <row r="23" spans="2:5">
@@ -1750,7 +1820,7 @@
       </c>
       <c r="D23" s="9"/>
       <c r="E23" s="10" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
     </row>
     <row r="24" spans="2:5">
@@ -1762,7 +1832,7 @@
       </c>
       <c r="D24" s="6"/>
       <c r="E24" s="7" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="25" spans="2:5">
@@ -1773,7 +1843,7 @@
         <v>19</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="E25" s="7"/>
     </row>
@@ -1785,7 +1855,7 @@
         <v>19</v>
       </c>
       <c r="D26" s="6" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="E26" s="7"/>
     </row>
@@ -1797,7 +1867,7 @@
         <v>19</v>
       </c>
       <c r="D27" s="6" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="E27" s="7"/>
     </row>
@@ -1809,52 +1879,52 @@
         <v>19</v>
       </c>
       <c r="D28" s="20" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="E28" s="7" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
     </row>
     <row r="29" spans="2:5">
       <c r="B29" s="5" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="C29" s="6" t="s">
         <v>19</v>
       </c>
       <c r="D29" s="6" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="E29" s="7" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
     </row>
     <row r="30" spans="2:5">
       <c r="B30" s="5" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="C30" s="6" t="s">
         <v>19</v>
       </c>
       <c r="D30" s="6" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="E30" s="7" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
     </row>
     <row r="31" spans="2:5">
       <c r="B31" s="5" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="C31" s="6" t="s">
         <v>19</v>
       </c>
       <c r="D31" s="6" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="E31" s="7" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
     </row>
     <row r="32" spans="2:5">
@@ -1865,36 +1935,36 @@
         <v>19</v>
       </c>
       <c r="D32" s="6" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="E32" s="7"/>
     </row>
     <row r="33" spans="2:5">
       <c r="B33" s="5" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="C33" s="6" t="s">
         <v>19</v>
       </c>
       <c r="D33" s="6" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="E33" s="7" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
     </row>
     <row r="34" spans="2:5">
       <c r="B34" s="5" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="C34" s="6" t="s">
         <v>19</v>
       </c>
       <c r="D34" s="6" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="E34" s="7" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
     </row>
     <row r="35" spans="2:5">
@@ -1905,7 +1975,7 @@
         <v>19</v>
       </c>
       <c r="D35" s="6" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="E35" s="7"/>
     </row>
@@ -1917,7 +1987,7 @@
         <v>19</v>
       </c>
       <c r="D36" s="6" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="E36" s="7"/>
     </row>
@@ -1930,7 +2000,7 @@
       </c>
       <c r="D37" s="12"/>
       <c r="E37" s="13" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="38" spans="2:5">
@@ -1942,7 +2012,7 @@
       </c>
       <c r="D38" s="12"/>
       <c r="E38" s="13" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="39" spans="2:5">
@@ -1954,7 +2024,7 @@
       </c>
       <c r="D39" s="12"/>
       <c r="E39" s="13" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row r="40" spans="2:5">
@@ -1966,7 +2036,7 @@
       </c>
       <c r="D40" s="12"/>
       <c r="E40" s="13" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="41" spans="2:5">
@@ -1974,13 +2044,13 @@
         <v>31</v>
       </c>
       <c r="C41" s="15" t="s">
+        <v>94</v>
+      </c>
+      <c r="D41" s="15" t="s">
         <v>93</v>
       </c>
-      <c r="D41" s="15" t="s">
+      <c r="E41" s="16" t="s">
         <v>92</v>
-      </c>
-      <c r="E41" s="16" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="42" spans="2:5">
@@ -1988,11 +2058,11 @@
         <v>32</v>
       </c>
       <c r="C42" s="6" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D42" s="6"/>
       <c r="E42" s="7" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
     <row r="43" spans="2:5">
@@ -2000,11 +2070,11 @@
         <v>33</v>
       </c>
       <c r="C43" s="6" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D43" s="6"/>
       <c r="E43" s="7" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
     <row r="44" spans="2:5">
@@ -2012,11 +2082,11 @@
         <v>34</v>
       </c>
       <c r="C44" s="6" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D44" s="6"/>
       <c r="E44" s="7" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
     <row r="45" spans="2:5">
@@ -2024,11 +2094,11 @@
         <v>35</v>
       </c>
       <c r="C45" s="9" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D45" s="9"/>
       <c r="E45" s="10" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
     <row r="46" spans="2:5">
@@ -2040,7 +2110,7 @@
       </c>
       <c r="D46" s="12"/>
       <c r="E46" s="13" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="47" spans="2:5">
@@ -2052,7 +2122,7 @@
       </c>
       <c r="D47" s="9"/>
       <c r="E47" s="10" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="48" spans="2:5">
@@ -2091,10 +2161,10 @@
       </c>
       <c r="C51" s="12"/>
       <c r="D51" s="12" t="s">
+        <v>98</v>
+      </c>
+      <c r="E51" s="13" t="s">
         <v>97</v>
-      </c>
-      <c r="E51" s="13" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="52" spans="2:5">
@@ -2106,7 +2176,7 @@
       </c>
       <c r="D52" s="15"/>
       <c r="E52" s="16" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
     </row>
     <row r="53" spans="2:5">
@@ -2128,7 +2198,7 @@
       </c>
       <c r="D54" s="6"/>
       <c r="E54" s="7" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
     </row>
     <row r="55" spans="2:5">
@@ -2150,7 +2220,7 @@
       </c>
       <c r="D56" s="15"/>
       <c r="E56" s="16" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
     </row>
     <row r="57" spans="2:5">
@@ -2172,7 +2242,7 @@
       </c>
       <c r="D58" s="6"/>
       <c r="E58" s="7" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
     </row>
     <row r="59" spans="2:5">
@@ -2194,7 +2264,7 @@
       </c>
       <c r="D60" s="12"/>
       <c r="E60" s="13" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
     </row>
     <row r="61" spans="2:5">
@@ -2206,7 +2276,7 @@
       </c>
       <c r="D61" s="12"/>
       <c r="E61" s="13" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
     </row>
     <row r="62" spans="2:5">
@@ -2218,7 +2288,7 @@
       </c>
       <c r="D62" s="12"/>
       <c r="E62" s="13" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
     </row>
     <row r="63" spans="2:5">
@@ -2228,7 +2298,7 @@
       <c r="C63" s="12"/>
       <c r="D63" s="12"/>
       <c r="E63" s="13" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
     </row>
     <row r="64" spans="2:5">
@@ -2240,7 +2310,7 @@
       </c>
       <c r="D64" s="12"/>
       <c r="E64" s="13" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
     </row>
     <row r="65" spans="2:5">
@@ -2252,7 +2322,7 @@
       </c>
       <c r="D65" s="12"/>
       <c r="E65" s="13" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
     </row>
     <row r="66" spans="2:5">
@@ -2264,7 +2334,7 @@
       </c>
       <c r="D66" s="12"/>
       <c r="E66" s="13" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
     </row>
     <row r="67" spans="2:5">
@@ -2292,11 +2362,11 @@
         <v>59</v>
       </c>
       <c r="C69" s="15" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="D69" s="15"/>
       <c r="E69" s="16" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
     </row>
     <row r="70" spans="2:5">
@@ -2304,11 +2374,11 @@
         <v>60</v>
       </c>
       <c r="C70" s="9" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="D70" s="9"/>
       <c r="E70" s="10" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
     </row>
     <row r="71" spans="2:5">
@@ -2452,7 +2522,7 @@
       </c>
       <c r="D84" s="22"/>
       <c r="E84" s="23" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
     </row>
   </sheetData>
@@ -2466,7 +2536,7 @@
   <dimension ref="B3:E53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E35" sqref="E35"/>
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2485,7 +2555,7 @@
         <v>79</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>81</v>
@@ -2494,19 +2564,19 @@
     <row r="4" spans="2:5" ht="15.75" thickBot="1"/>
     <row r="5" spans="2:5">
       <c r="B5" s="2" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="3" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
     </row>
     <row r="6" spans="2:5">
       <c r="B6" s="5" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C6" s="6"/>
       <c r="D6" s="6"/>
@@ -2514,7 +2584,7 @@
     </row>
     <row r="7" spans="2:5">
       <c r="B7" s="5" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C7" s="6"/>
       <c r="D7" s="6"/>
@@ -2522,514 +2592,508 @@
     </row>
     <row r="8" spans="2:5">
       <c r="B8" s="11" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="D8" s="12"/>
       <c r="E8" s="13" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
     </row>
     <row r="9" spans="2:5">
       <c r="B9" s="11" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="D9" s="12"/>
       <c r="E9" s="13" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
     </row>
     <row r="10" spans="2:5">
       <c r="B10" s="11" t="s">
-        <v>103</v>
-      </c>
-      <c r="C10" s="12"/>
+        <v>104</v>
+      </c>
+      <c r="C10" s="12" t="s">
+        <v>104</v>
+      </c>
       <c r="D10" s="12" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="E10" s="13"/>
     </row>
     <row r="11" spans="2:5">
       <c r="B11" s="11" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D11" s="12"/>
       <c r="E11" s="13"/>
     </row>
     <row r="12" spans="2:5">
       <c r="B12" s="11" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="D12" s="12"/>
       <c r="E12" s="13"/>
     </row>
     <row r="13" spans="2:5">
       <c r="B13" s="11" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="D13" s="12"/>
       <c r="E13" s="13"/>
     </row>
     <row r="14" spans="2:5">
       <c r="B14" s="11" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="D14" s="12"/>
       <c r="E14" s="13"/>
     </row>
     <row r="15" spans="2:5">
       <c r="B15" s="11" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C15" s="24" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="D15" s="12"/>
       <c r="E15" s="13" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
     </row>
     <row r="16" spans="2:5">
       <c r="B16" s="11" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C16" s="12"/>
       <c r="D16" s="12"/>
       <c r="E16" s="13" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
     </row>
     <row r="17" spans="2:5">
       <c r="B17" s="11" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C17" s="12" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="D17" s="12"/>
       <c r="E17" s="13" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
     </row>
     <row r="18" spans="2:5">
       <c r="B18" s="11" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C18" s="12" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="D18" s="12"/>
       <c r="E18" s="13" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
     </row>
     <row r="19" spans="2:5">
       <c r="B19" s="11" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C19" s="12" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="D19" s="12"/>
       <c r="E19" s="13" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
     </row>
     <row r="20" spans="2:5">
       <c r="B20" s="11" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C20" s="12" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="D20" s="12"/>
       <c r="E20" s="13" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
     </row>
     <row r="21" spans="2:5">
       <c r="B21" s="11" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="C21" s="12" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="D21" s="12"/>
       <c r="E21" s="13" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
     </row>
     <row r="22" spans="2:5">
       <c r="B22" s="11" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C22" s="12"/>
       <c r="D22" s="12" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="E22" s="13" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
     </row>
     <row r="23" spans="2:5">
       <c r="B23" s="11" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C23" s="12"/>
       <c r="D23" s="12"/>
       <c r="E23" s="13" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
     </row>
     <row r="24" spans="2:5">
       <c r="B24" s="11" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C24" s="12" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="D24" s="12"/>
       <c r="E24" s="13" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
     </row>
     <row r="25" spans="2:5">
       <c r="B25" s="11" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C25" s="12" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="D25" s="12"/>
       <c r="E25" s="13" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
     </row>
     <row r="26" spans="2:5">
       <c r="B26" s="5" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="C26" s="6"/>
       <c r="D26" s="6"/>
       <c r="E26" s="7" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
     </row>
     <row r="27" spans="2:5">
       <c r="B27" s="5" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C27" s="6"/>
       <c r="D27" s="6"/>
       <c r="E27" s="7" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
     </row>
     <row r="28" spans="2:5">
       <c r="B28" s="5" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C28" s="6"/>
       <c r="D28" s="6"/>
       <c r="E28" s="7" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
     </row>
     <row r="29" spans="2:5">
       <c r="B29" s="5" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C29" s="6"/>
       <c r="D29" s="6"/>
       <c r="E29" s="7" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
     </row>
     <row r="30" spans="2:5">
       <c r="B30" s="5" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C30" s="6"/>
       <c r="D30" s="6"/>
       <c r="E30" s="7" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
     </row>
     <row r="31" spans="2:5">
       <c r="B31" s="5" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C31" s="6"/>
       <c r="D31" s="6"/>
       <c r="E31" s="7" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
     </row>
     <row r="32" spans="2:5">
       <c r="B32" s="5" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="C32" s="6"/>
       <c r="D32" s="6"/>
       <c r="E32" s="7" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
     </row>
     <row r="33" spans="2:5">
       <c r="B33" s="5" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="C33" s="6" t="s">
+        <v>236</v>
+      </c>
+      <c r="D33" s="6" t="s">
         <v>234</v>
       </c>
-      <c r="D33" s="6" t="s">
-        <v>232</v>
-      </c>
       <c r="E33" s="7" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="34" spans="2:5">
+      <c r="B34" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="C34" s="6"/>
+      <c r="D34" s="6"/>
+      <c r="E34" s="7" t="s">
         <v>233</v>
-      </c>
-    </row>
-    <row r="34" spans="2:5">
-      <c r="B34" s="11" t="s">
-        <v>127</v>
-      </c>
-      <c r="C34" s="12" t="s">
-        <v>127</v>
-      </c>
-      <c r="D34" s="12"/>
-      <c r="E34" s="13" t="s">
-        <v>231</v>
       </c>
     </row>
     <row r="35" spans="2:5">
       <c r="B35" s="11" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="C35" s="12"/>
       <c r="D35" s="12"/>
       <c r="E35" s="13" t="s">
-        <v>279</v>
+        <v>149</v>
       </c>
     </row>
     <row r="36" spans="2:5">
       <c r="B36" s="11" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="C36" s="12" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="D36" s="12"/>
       <c r="E36" s="13" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
     </row>
     <row r="37" spans="2:5">
       <c r="B37" s="11" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C37" s="12" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="D37" s="12"/>
       <c r="E37" s="13" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
     </row>
     <row r="38" spans="2:5">
       <c r="B38" s="11" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="C38" s="12" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="D38" s="12"/>
       <c r="E38" s="13" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
     </row>
     <row r="39" spans="2:5">
       <c r="B39" s="11" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C39" s="12" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="D39" s="12"/>
       <c r="E39" s="13" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
     </row>
     <row r="40" spans="2:5">
       <c r="B40" s="11" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="C40" s="12" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="D40" s="12"/>
       <c r="E40" s="13"/>
     </row>
     <row r="41" spans="2:5">
       <c r="B41" s="11" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="C41" s="12"/>
       <c r="D41" s="12" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="E41" s="13" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
     </row>
     <row r="42" spans="2:5">
       <c r="B42" s="11" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="C42" s="12"/>
       <c r="D42" s="12"/>
       <c r="E42" s="13" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
     </row>
     <row r="43" spans="2:5">
       <c r="B43" s="11" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="C43" s="12" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="D43" s="12" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="E43" s="13" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
     </row>
     <row r="44" spans="2:5">
       <c r="B44" s="11" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C44" s="12" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="D44" s="12"/>
       <c r="E44" s="13" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
     </row>
     <row r="45" spans="2:5">
       <c r="B45" s="5" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="C45" s="6" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="D45" s="6"/>
       <c r="E45" s="7"/>
     </row>
     <row r="46" spans="2:5">
       <c r="B46" s="5" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="C46" s="6" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="D46" s="6"/>
       <c r="E46" s="7"/>
     </row>
     <row r="47" spans="2:5">
       <c r="B47" s="5" t="s">
-        <v>140</v>
-      </c>
-      <c r="C47" s="6" t="s">
-        <v>139</v>
-      </c>
+        <v>141</v>
+      </c>
+      <c r="C47" s="6"/>
       <c r="D47" s="6"/>
       <c r="E47" s="7" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
     </row>
     <row r="48" spans="2:5">
       <c r="B48" s="5" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="C48" s="6" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="D48" s="6"/>
       <c r="E48" s="7"/>
     </row>
     <row r="49" spans="2:5">
       <c r="B49" s="5" t="s">
-        <v>142</v>
-      </c>
-      <c r="C49" s="6" t="s">
-        <v>141</v>
-      </c>
+        <v>143</v>
+      </c>
+      <c r="C49" s="6"/>
       <c r="D49" s="6"/>
       <c r="E49" s="7" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
     </row>
     <row r="50" spans="2:5">
       <c r="B50" s="5" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C50" s="6" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="D50" s="6"/>
       <c r="E50" s="7"/>
     </row>
     <row r="51" spans="2:5">
       <c r="B51" s="11" t="s">
-        <v>144</v>
-      </c>
-      <c r="C51" s="6" t="s">
-        <v>143</v>
-      </c>
+        <v>145</v>
+      </c>
+      <c r="C51" s="12"/>
       <c r="D51" s="12"/>
       <c r="E51" s="13" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
     </row>
     <row r="52" spans="2:5">
       <c r="B52" s="11" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="C52" s="12"/>
       <c r="D52" s="12"/>
       <c r="E52" s="13" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
     </row>
     <row r="53" spans="2:5" ht="15.75" thickBot="1">
       <c r="B53" s="21" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="C53" s="22"/>
       <c r="D53" s="22" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="E53" s="23" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
     </row>
   </sheetData>
@@ -3043,10 +3107,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B3:E42"/>
+  <dimension ref="B3:E44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:XFD8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3064,7 +3128,7 @@
         <v>79</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>81</v>
@@ -3073,346 +3137,358 @@
     <row r="4" spans="2:5" ht="15.75" thickBot="1"/>
     <row r="5" spans="2:5">
       <c r="B5" s="25" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="C5" s="26" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="D5" s="26" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="E5" s="27" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
     </row>
     <row r="6" spans="2:5">
       <c r="B6" s="11" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="D6" s="12"/>
       <c r="E6" s="13" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
     </row>
     <row r="7" spans="2:5">
       <c r="B7" s="5" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="D7" s="6"/>
       <c r="E7" s="7" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
     </row>
     <row r="8" spans="2:5">
       <c r="B8" s="5" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="D8" s="6"/>
       <c r="E8" s="10" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
     </row>
     <row r="9" spans="2:5">
       <c r="B9" s="14" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="C9" s="15" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="D9" s="15"/>
       <c r="E9" s="16"/>
     </row>
     <row r="10" spans="2:5">
       <c r="B10" s="5" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="D10" s="6"/>
       <c r="E10" s="7" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="11" spans="2:5">
       <c r="B11" s="5" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="D11" s="6"/>
       <c r="E11" s="7"/>
     </row>
     <row r="12" spans="2:5">
       <c r="B12" s="8" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="D12" s="9"/>
       <c r="E12" s="10" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
     </row>
     <row r="13" spans="2:5">
       <c r="B13" s="5" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="D13" s="6"/>
       <c r="E13" s="7" t="s">
-        <v>267</v>
+        <v>269</v>
       </c>
     </row>
     <row r="14" spans="2:5">
       <c r="B14" s="5" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="D14" s="6"/>
       <c r="E14" s="7"/>
     </row>
     <row r="15" spans="2:5">
-      <c r="B15" s="11" t="s">
-        <v>182</v>
-      </c>
-      <c r="C15" s="12" t="s">
-        <v>182</v>
-      </c>
-      <c r="D15" s="12"/>
-      <c r="E15" s="13"/>
+      <c r="B15" s="5" t="s">
+        <v>273</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>258</v>
+      </c>
+      <c r="D15" s="6"/>
+      <c r="E15" s="7"/>
     </row>
     <row r="16" spans="2:5">
       <c r="B16" s="11" t="s">
-        <v>169</v>
-      </c>
-      <c r="C16" s="6" t="s">
-        <v>170</v>
-      </c>
-      <c r="D16" s="12" t="s">
-        <v>193</v>
-      </c>
+        <v>276</v>
+      </c>
+      <c r="C16" s="12" t="s">
+        <v>276</v>
+      </c>
+      <c r="D16" s="12"/>
       <c r="E16" s="13" t="s">
-        <v>194</v>
+        <v>277</v>
       </c>
     </row>
     <row r="17" spans="2:5">
-      <c r="B17" s="5" t="s">
-        <v>173</v>
-      </c>
-      <c r="C17" s="6" t="s">
-        <v>173</v>
-      </c>
-      <c r="D17" s="6"/>
-      <c r="E17" s="7"/>
+      <c r="B17" s="11" t="s">
+        <v>184</v>
+      </c>
+      <c r="C17" s="12" t="s">
+        <v>184</v>
+      </c>
+      <c r="D17" s="12" t="s">
+        <v>272</v>
+      </c>
+      <c r="E17" s="13" t="s">
+        <v>271</v>
+      </c>
     </row>
     <row r="18" spans="2:5">
       <c r="B18" s="11" t="s">
-        <v>183</v>
-      </c>
-      <c r="C18" s="12" t="s">
-        <v>183</v>
-      </c>
-      <c r="D18" s="12"/>
+        <v>171</v>
+      </c>
+      <c r="C18" s="12"/>
+      <c r="D18" s="12" t="s">
+        <v>195</v>
+      </c>
       <c r="E18" s="13" t="s">
-        <v>189</v>
+        <v>196</v>
       </c>
     </row>
     <row r="19" spans="2:5">
-      <c r="B19" s="11" t="s">
-        <v>186</v>
-      </c>
-      <c r="C19" s="12" t="s">
-        <v>186</v>
-      </c>
-      <c r="D19" s="12"/>
-      <c r="E19" s="13" t="s">
-        <v>190</v>
-      </c>
+      <c r="B19" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>175</v>
+      </c>
+      <c r="D19" s="6"/>
+      <c r="E19" s="7"/>
     </row>
     <row r="20" spans="2:5">
-      <c r="B20" s="14" t="s">
-        <v>178</v>
-      </c>
-      <c r="C20" s="15"/>
-      <c r="D20" s="15" t="s">
+      <c r="B20" s="11" t="s">
+        <v>185</v>
+      </c>
+      <c r="C20" s="12" t="s">
+        <v>185</v>
+      </c>
+      <c r="D20" s="12"/>
+      <c r="E20" s="13" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5">
+      <c r="B21" s="11" t="s">
+        <v>188</v>
+      </c>
+      <c r="C21" s="12" t="s">
+        <v>188</v>
+      </c>
+      <c r="D21" s="12"/>
+      <c r="E21" s="13" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5">
+      <c r="B22" s="14" t="s">
+        <v>180</v>
+      </c>
+      <c r="C22" s="15"/>
+      <c r="D22" s="15" t="s">
+        <v>195</v>
+      </c>
+      <c r="E22" s="16" t="s">
         <v>193</v>
       </c>
-      <c r="E20" s="16" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="21" spans="2:5">
-      <c r="B21" s="8" t="s">
-        <v>179</v>
-      </c>
-      <c r="C21" s="9"/>
-      <c r="D21" s="9" t="s">
-        <v>193</v>
-      </c>
-      <c r="E21" s="10" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="22" spans="2:5">
-      <c r="B22" s="5" t="s">
-        <v>177</v>
-      </c>
-      <c r="C22" s="6" t="s">
-        <v>177</v>
-      </c>
-      <c r="D22" s="6"/>
-      <c r="E22" s="7"/>
     </row>
     <row r="23" spans="2:5">
-      <c r="B23" s="5" t="s">
-        <v>165</v>
-      </c>
-      <c r="C23" s="6" t="s">
-        <v>165</v>
-      </c>
-      <c r="D23" s="6"/>
-      <c r="E23" s="7"/>
+      <c r="B23" s="8" t="s">
+        <v>181</v>
+      </c>
+      <c r="C23" s="9"/>
+      <c r="D23" s="9" t="s">
+        <v>195</v>
+      </c>
+      <c r="E23" s="10" t="s">
+        <v>194</v>
+      </c>
     </row>
     <row r="24" spans="2:5">
       <c r="B24" s="5" t="s">
-        <v>174</v>
+        <v>179</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>173</v>
+        <v>179</v>
       </c>
       <c r="D24" s="6"/>
-      <c r="E24" s="7" t="s">
-        <v>150</v>
-      </c>
+      <c r="E24" s="7"/>
     </row>
     <row r="25" spans="2:5">
       <c r="B25" s="5" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="D25" s="6"/>
       <c r="E25" s="7"/>
     </row>
     <row r="26" spans="2:5">
       <c r="B26" s="5" t="s">
-        <v>185</v>
+        <v>176</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>170</v>
-      </c>
-      <c r="D26" s="6"/>
-      <c r="E26" s="7"/>
+        <v>176</v>
+      </c>
+      <c r="D26" s="6" t="s">
+        <v>272</v>
+      </c>
+      <c r="E26" s="7" t="s">
+        <v>271</v>
+      </c>
     </row>
     <row r="27" spans="2:5">
       <c r="B27" s="5" t="s">
-        <v>187</v>
+        <v>166</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>187</v>
+        <v>175</v>
       </c>
       <c r="D27" s="6"/>
       <c r="E27" s="7"/>
     </row>
     <row r="28" spans="2:5">
       <c r="B28" s="5" t="s">
-        <v>170</v>
-      </c>
-      <c r="C28" s="6" t="s">
-        <v>170</v>
-      </c>
-      <c r="D28" s="6"/>
-      <c r="E28" s="7"/>
+        <v>187</v>
+      </c>
+      <c r="C28" s="6"/>
+      <c r="D28" s="6" t="s">
+        <v>195</v>
+      </c>
+      <c r="E28" s="7" t="s">
+        <v>274</v>
+      </c>
     </row>
     <row r="29" spans="2:5">
       <c r="B29" s="5" t="s">
-        <v>162</v>
-      </c>
-      <c r="C29" s="6" t="s">
-        <v>162</v>
-      </c>
-      <c r="D29" s="6"/>
-      <c r="E29" s="7"/>
+        <v>189</v>
+      </c>
+      <c r="C29" s="6"/>
+      <c r="D29" s="6" t="s">
+        <v>272</v>
+      </c>
+      <c r="E29" s="7" t="s">
+        <v>271</v>
+      </c>
     </row>
     <row r="30" spans="2:5">
       <c r="B30" s="5" t="s">
-        <v>188</v>
+        <v>172</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>188</v>
+        <v>164</v>
       </c>
       <c r="D30" s="6"/>
       <c r="E30" s="7"/>
     </row>
     <row r="31" spans="2:5">
-      <c r="B31" s="11" t="s">
-        <v>152</v>
-      </c>
-      <c r="C31" s="12"/>
-      <c r="D31" s="12"/>
-      <c r="E31" s="13" t="s">
-        <v>258</v>
-      </c>
+      <c r="B31" s="5" t="s">
+        <v>164</v>
+      </c>
+      <c r="C31" s="6" t="s">
+        <v>164</v>
+      </c>
+      <c r="D31" s="6"/>
+      <c r="E31" s="7"/>
     </row>
     <row r="32" spans="2:5">
-      <c r="B32" s="14" t="s">
-        <v>172</v>
-      </c>
-      <c r="C32" s="15" t="s">
-        <v>265</v>
-      </c>
-      <c r="D32" s="15"/>
-      <c r="E32" s="16" t="s">
-        <v>259</v>
+      <c r="B32" s="8" t="s">
+        <v>190</v>
+      </c>
+      <c r="C32" s="9" t="s">
+        <v>190</v>
+      </c>
+      <c r="D32" s="9" t="s">
+        <v>195</v>
+      </c>
+      <c r="E32" s="10" t="s">
+        <v>275</v>
       </c>
     </row>
     <row r="33" spans="2:5">
-      <c r="B33" s="5" t="s">
-        <v>163</v>
-      </c>
-      <c r="C33" s="6" t="s">
-        <v>265</v>
-      </c>
-      <c r="D33" s="6"/>
-      <c r="E33" s="7" t="s">
+      <c r="B33" s="11" t="s">
+        <v>154</v>
+      </c>
+      <c r="C33" s="12"/>
+      <c r="D33" s="12" t="s">
+        <v>195</v>
+      </c>
+      <c r="E33" s="13" t="s">
         <v>260</v>
       </c>
     </row>
     <row r="34" spans="2:5">
-      <c r="B34" s="5" t="s">
-        <v>168</v>
-      </c>
-      <c r="C34" s="6" t="s">
-        <v>265</v>
-      </c>
-      <c r="D34" s="6"/>
-      <c r="E34" s="7" t="s">
+      <c r="B34" s="14" t="s">
+        <v>174</v>
+      </c>
+      <c r="C34" s="15" t="s">
+        <v>267</v>
+      </c>
+      <c r="D34" s="15"/>
+      <c r="E34" s="16" t="s">
         <v>261</v>
       </c>
     </row>
     <row r="35" spans="2:5">
       <c r="B35" s="5" t="s">
-        <v>161</v>
+        <v>165</v>
       </c>
       <c r="C35" s="6" t="s">
-        <v>265</v>
+        <v>267</v>
       </c>
       <c r="D35" s="6"/>
       <c r="E35" s="7" t="s">
@@ -3421,10 +3497,10 @@
     </row>
     <row r="36" spans="2:5">
       <c r="B36" s="5" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
       <c r="C36" s="6" t="s">
-        <v>265</v>
+        <v>267</v>
       </c>
       <c r="D36" s="6"/>
       <c r="E36" s="7" t="s">
@@ -3432,78 +3508,455 @@
       </c>
     </row>
     <row r="37" spans="2:5">
-      <c r="B37" s="8" t="s">
-        <v>151</v>
-      </c>
-      <c r="C37" s="9" t="s">
-        <v>265</v>
-      </c>
-      <c r="D37" s="9"/>
-      <c r="E37" s="10" t="s">
+      <c r="B37" s="5" t="s">
+        <v>163</v>
+      </c>
+      <c r="C37" s="6" t="s">
+        <v>267</v>
+      </c>
+      <c r="D37" s="6"/>
+      <c r="E37" s="7" t="s">
         <v>264</v>
       </c>
     </row>
     <row r="38" spans="2:5">
       <c r="B38" s="5" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C38" s="6" t="s">
-        <v>184</v>
+        <v>267</v>
       </c>
       <c r="D38" s="6"/>
-      <c r="E38" s="7"/>
+      <c r="E38" s="7" t="s">
+        <v>265</v>
+      </c>
     </row>
     <row r="39" spans="2:5">
-      <c r="B39" s="5" t="s">
-        <v>154</v>
-      </c>
-      <c r="C39" s="6" t="s">
-        <v>184</v>
-      </c>
-      <c r="D39" s="6"/>
-      <c r="E39" s="7" t="s">
+      <c r="B39" s="8" t="s">
+        <v>153</v>
+      </c>
+      <c r="C39" s="9" t="s">
+        <v>267</v>
+      </c>
+      <c r="D39" s="9"/>
+      <c r="E39" s="10" t="s">
         <v>266</v>
       </c>
     </row>
     <row r="40" spans="2:5">
       <c r="B40" s="5" t="s">
-        <v>159</v>
+        <v>186</v>
       </c>
       <c r="C40" s="6" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="D40" s="6"/>
       <c r="E40" s="7"/>
     </row>
     <row r="41" spans="2:5">
       <c r="B41" s="5" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="C41" s="6" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="D41" s="6"/>
-      <c r="E41" s="7"/>
-    </row>
-    <row r="42" spans="2:5" ht="15.75" thickBot="1">
-      <c r="B42" s="17" t="s">
-        <v>171</v>
+      <c r="E41" s="7" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="42" spans="2:5">
+      <c r="B42" s="5" t="s">
+        <v>161</v>
       </c>
       <c r="C42" s="6" t="s">
-        <v>184</v>
-      </c>
-      <c r="D42" s="18"/>
-      <c r="E42" s="19"/>
+        <v>186</v>
+      </c>
+      <c r="D42" s="6"/>
+      <c r="E42" s="7"/>
+    </row>
+    <row r="43" spans="2:5">
+      <c r="B43" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="C43" s="6" t="s">
+        <v>186</v>
+      </c>
+      <c r="D43" s="6"/>
+      <c r="E43" s="7"/>
+    </row>
+    <row r="44" spans="2:5" ht="15.75" thickBot="1">
+      <c r="B44" s="17" t="s">
+        <v>173</v>
+      </c>
+      <c r="C44" s="18" t="s">
+        <v>186</v>
+      </c>
+      <c r="D44" s="18"/>
+      <c r="E44" s="19"/>
     </row>
   </sheetData>
   <sortState ref="B5:E42">
     <sortCondition ref="B5"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="B3:E44"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="3" width="28.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="86.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:5" s="1" customFormat="1" ht="18.75">
+      <c r="B3" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" ht="15.75" thickBot="1"/>
+    <row r="5" spans="2:5">
+      <c r="B5" s="2" t="s">
+        <v>278</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>278</v>
+      </c>
+      <c r="D5" s="3"/>
+      <c r="E5" s="4" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5">
+      <c r="B6" s="5" t="s">
+        <v>279</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>279</v>
+      </c>
+      <c r="D6" s="6"/>
+      <c r="E6" s="7" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5">
+      <c r="B7" s="5" t="s">
+        <v>280</v>
+      </c>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6" t="s">
+        <v>291</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5">
+      <c r="B8" s="5" t="s">
+        <v>281</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>281</v>
+      </c>
+      <c r="D8" s="6"/>
+      <c r="E8" s="7" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5">
+      <c r="B9" s="5" t="s">
+        <v>282</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>282</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>291</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5">
+      <c r="B10" s="5" t="s">
+        <v>283</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>283</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>291</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5">
+      <c r="B11" s="5" t="s">
+        <v>284</v>
+      </c>
+      <c r="C11" s="6"/>
+      <c r="D11" s="6" t="s">
+        <v>291</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5">
+      <c r="B12" s="5" t="s">
+        <v>285</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>285</v>
+      </c>
+      <c r="D12" s="6"/>
+      <c r="E12" s="7" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="13" spans="2:5">
+      <c r="B13" s="5" t="s">
+        <v>286</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>286</v>
+      </c>
+      <c r="D13" s="6"/>
+      <c r="E13" s="7" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="14" spans="2:5">
+      <c r="B14" s="5" t="s">
+        <v>287</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>287</v>
+      </c>
+      <c r="D14" s="6"/>
+      <c r="E14" s="7" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="15" spans="2:5">
+      <c r="B15" s="5" t="s">
+        <v>288</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>288</v>
+      </c>
+      <c r="D15" s="6"/>
+      <c r="E15" s="7" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="16" spans="2:5" ht="15.75" thickBot="1">
+      <c r="B16" s="17" t="s">
+        <v>289</v>
+      </c>
+      <c r="C16" s="18" t="s">
+        <v>289</v>
+      </c>
+      <c r="D16" s="18"/>
+      <c r="E16" s="19" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5">
+      <c r="B17" s="3"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+    </row>
+    <row r="18" spans="2:5">
+      <c r="B18" s="6"/>
+      <c r="C18" s="6"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="6"/>
+    </row>
+    <row r="19" spans="2:5">
+      <c r="B19" s="6"/>
+      <c r="C19" s="6"/>
+      <c r="D19" s="6"/>
+      <c r="E19" s="6"/>
+    </row>
+    <row r="20" spans="2:5">
+      <c r="B20" s="6"/>
+      <c r="C20" s="6"/>
+      <c r="D20" s="6"/>
+      <c r="E20" s="6"/>
+    </row>
+    <row r="21" spans="2:5">
+      <c r="B21" s="6"/>
+      <c r="C21" s="6"/>
+      <c r="D21" s="6"/>
+      <c r="E21" s="6"/>
+    </row>
+    <row r="22" spans="2:5">
+      <c r="B22" s="6"/>
+      <c r="C22" s="6"/>
+      <c r="D22" s="6"/>
+      <c r="E22" s="6"/>
+    </row>
+    <row r="23" spans="2:5">
+      <c r="B23" s="6"/>
+      <c r="C23" s="6"/>
+      <c r="D23" s="6"/>
+      <c r="E23" s="6"/>
+    </row>
+    <row r="24" spans="2:5">
+      <c r="B24" s="6"/>
+      <c r="C24" s="6"/>
+      <c r="D24" s="6"/>
+      <c r="E24" s="6"/>
+    </row>
+    <row r="25" spans="2:5">
+      <c r="B25" s="6"/>
+      <c r="C25" s="6"/>
+      <c r="D25" s="6"/>
+      <c r="E25" s="6"/>
+    </row>
+    <row r="26" spans="2:5">
+      <c r="B26" s="6"/>
+      <c r="C26" s="6"/>
+      <c r="D26" s="6"/>
+      <c r="E26" s="6"/>
+    </row>
+    <row r="27" spans="2:5">
+      <c r="B27" s="6"/>
+      <c r="C27" s="6"/>
+      <c r="D27" s="6"/>
+      <c r="E27" s="6"/>
+    </row>
+    <row r="28" spans="2:5">
+      <c r="B28" s="6"/>
+      <c r="C28" s="6"/>
+      <c r="D28" s="6"/>
+      <c r="E28" s="6"/>
+    </row>
+    <row r="29" spans="2:5">
+      <c r="B29" s="6"/>
+      <c r="C29" s="6"/>
+      <c r="D29" s="6"/>
+      <c r="E29" s="6"/>
+    </row>
+    <row r="30" spans="2:5">
+      <c r="B30" s="6"/>
+      <c r="C30" s="6"/>
+      <c r="D30" s="6"/>
+      <c r="E30" s="6"/>
+    </row>
+    <row r="31" spans="2:5">
+      <c r="B31" s="6"/>
+      <c r="C31" s="6"/>
+      <c r="D31" s="6"/>
+      <c r="E31" s="6"/>
+    </row>
+    <row r="32" spans="2:5">
+      <c r="B32" s="6"/>
+      <c r="C32" s="6"/>
+      <c r="D32" s="6"/>
+      <c r="E32" s="6"/>
+    </row>
+    <row r="33" spans="2:5">
+      <c r="B33" s="6"/>
+      <c r="C33" s="6"/>
+      <c r="D33" s="6"/>
+      <c r="E33" s="6"/>
+    </row>
+    <row r="34" spans="2:5">
+      <c r="B34" s="6"/>
+      <c r="C34" s="6"/>
+      <c r="D34" s="6"/>
+      <c r="E34" s="6"/>
+    </row>
+    <row r="35" spans="2:5">
+      <c r="B35" s="6"/>
+      <c r="C35" s="6"/>
+      <c r="D35" s="6"/>
+      <c r="E35" s="6"/>
+    </row>
+    <row r="36" spans="2:5">
+      <c r="B36" s="6"/>
+      <c r="C36" s="6"/>
+      <c r="D36" s="6"/>
+      <c r="E36" s="6"/>
+    </row>
+    <row r="37" spans="2:5">
+      <c r="B37" s="6"/>
+      <c r="C37" s="6"/>
+      <c r="D37" s="6"/>
+      <c r="E37" s="6"/>
+    </row>
+    <row r="38" spans="2:5">
+      <c r="B38" s="6"/>
+      <c r="C38" s="6"/>
+      <c r="D38" s="6"/>
+      <c r="E38" s="6"/>
+    </row>
+    <row r="39" spans="2:5">
+      <c r="B39" s="6"/>
+      <c r="C39" s="6"/>
+      <c r="D39" s="6"/>
+      <c r="E39" s="6"/>
+    </row>
+    <row r="40" spans="2:5">
+      <c r="B40" s="6"/>
+      <c r="C40" s="6"/>
+      <c r="D40" s="6"/>
+      <c r="E40" s="6"/>
+    </row>
+    <row r="41" spans="2:5">
+      <c r="B41" s="6"/>
+      <c r="C41" s="6"/>
+      <c r="D41" s="6"/>
+      <c r="E41" s="6"/>
+    </row>
+    <row r="42" spans="2:5">
+      <c r="B42" s="6"/>
+      <c r="C42" s="6"/>
+      <c r="D42" s="6"/>
+      <c r="E42" s="6"/>
+    </row>
+    <row r="43" spans="2:5">
+      <c r="B43" s="6"/>
+      <c r="C43" s="6"/>
+      <c r="D43" s="6"/>
+      <c r="E43" s="6"/>
+    </row>
+    <row r="44" spans="2:5">
+      <c r="B44" s="6"/>
+      <c r="C44" s="6"/>
+      <c r="D44" s="6"/>
+      <c r="E44" s="6"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H18"/>
   <sheetViews>
@@ -3521,7 +3974,7 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="H1" t="s">
-        <v>285</v>
+        <v>309</v>
       </c>
     </row>
     <row r="2" spans="1:8">
@@ -3537,24 +3990,24 @@
     </row>
     <row r="3" spans="1:8">
       <c r="A3" t="s">
-        <v>280</v>
+        <v>308</v>
       </c>
       <c r="C3" t="s">
-        <v>270</v>
+        <v>307</v>
       </c>
       <c r="D3" s="29" t="s">
-        <v>273</v>
+        <v>306</v>
       </c>
       <c r="E3" s="29" t="s">
-        <v>274</v>
+        <v>305</v>
       </c>
       <c r="F3" s="28" t="s">
-        <v>275</v>
+        <v>304</v>
       </c>
     </row>
     <row r="4" spans="1:8">
       <c r="B4" t="s">
-        <v>269</v>
+        <v>303</v>
       </c>
       <c r="C4">
         <v>210</v>
@@ -3574,7 +4027,7 @@
     </row>
     <row r="5" spans="1:8">
       <c r="B5" t="s">
-        <v>272</v>
+        <v>302</v>
       </c>
       <c r="C5">
         <v>12</v>
@@ -3594,7 +4047,7 @@
     </row>
     <row r="6" spans="1:8">
       <c r="B6" t="s">
-        <v>271</v>
+        <v>301</v>
       </c>
       <c r="C6">
         <f>C4-(2*C5)</f>
@@ -3619,13 +4072,13 @@
     </row>
     <row r="8" spans="1:8">
       <c r="A8" t="s">
-        <v>283</v>
+        <v>300</v>
       </c>
       <c r="G8" s="28"/>
     </row>
     <row r="9" spans="1:8">
       <c r="B9" t="s">
-        <v>281</v>
+        <v>299</v>
       </c>
       <c r="C9">
         <v>186</v>
@@ -3637,22 +4090,22 @@
     </row>
     <row r="11" spans="1:8">
       <c r="A11" t="s">
-        <v>282</v>
+        <v>298</v>
       </c>
     </row>
     <row r="12" spans="1:8">
       <c r="B12" t="s">
-        <v>276</v>
+        <v>295</v>
       </c>
       <c r="C12">
         <v>35</v>
       </c>
       <c r="D12" s="29">
-        <f t="shared" ref="D12:D14" si="0">C12/$D$2</f>
+        <f>C12/$D$2</f>
         <v>1.3779527559055118</v>
       </c>
       <c r="E12" s="29">
-        <f t="shared" ref="E12:E14" si="1">D12*$E$2</f>
+        <f>D12*$E$2</f>
         <v>99.212598425196845</v>
       </c>
       <c r="F12" s="28">
@@ -3663,17 +4116,17 @@
     </row>
     <row r="13" spans="1:8">
       <c r="B13" t="s">
-        <v>277</v>
+        <v>294</v>
       </c>
       <c r="C13">
         <v>26</v>
       </c>
       <c r="D13" s="29">
-        <f t="shared" si="0"/>
+        <f>C13/$D$2</f>
         <v>1.0236220472440944</v>
       </c>
       <c r="E13" s="29">
-        <f t="shared" si="1"/>
+        <f>D13*$E$2</f>
         <v>73.7007874015748</v>
       </c>
       <c r="F13" s="28">
@@ -3684,18 +4137,18 @@
     </row>
     <row r="14" spans="1:8">
       <c r="B14" t="s">
-        <v>278</v>
+        <v>297</v>
       </c>
       <c r="C14">
         <f>C6-C13-C12</f>
         <v>125</v>
       </c>
       <c r="D14" s="29">
-        <f t="shared" si="0"/>
+        <f>C14/$D$2</f>
         <v>4.9212598425196852</v>
       </c>
       <c r="E14" s="29">
-        <f t="shared" si="1"/>
+        <f>D14*$E$2</f>
         <v>354.33070866141736</v>
       </c>
       <c r="F14" s="28">
@@ -3710,43 +4163,43 @@
     </row>
     <row r="16" spans="1:8">
       <c r="A16" t="s">
-        <v>284</v>
+        <v>296</v>
       </c>
     </row>
     <row r="17" spans="2:8">
       <c r="B17" t="s">
-        <v>276</v>
+        <v>295</v>
       </c>
       <c r="C17">
         <v>45</v>
       </c>
       <c r="D17" s="29">
-        <f t="shared" ref="D17:D18" si="2">C17/$D$2</f>
+        <f>C17/$D$2</f>
         <v>1.7716535433070868</v>
       </c>
       <c r="E17" s="29">
-        <f t="shared" ref="E17:E18" si="3">D17*$E$2</f>
+        <f>D17*$E$2</f>
         <v>127.55905511811025</v>
       </c>
       <c r="F17" s="28">
-        <f t="shared" ref="F17" si="4">E17*$F$2</f>
+        <f>E17*$F$2</f>
         <v>8359710.2362204734</v>
       </c>
     </row>
     <row r="18" spans="2:8">
       <c r="B18" t="s">
-        <v>277</v>
+        <v>294</v>
       </c>
       <c r="C18">
         <f>C6-C17</f>
         <v>141</v>
       </c>
       <c r="D18" s="29">
-        <f t="shared" si="2"/>
+        <f>C18/$D$2</f>
         <v>5.5511811023622046</v>
       </c>
       <c r="E18" s="29">
-        <f t="shared" si="3"/>
+        <f>D18*$E$2</f>
         <v>399.68503937007875</v>
       </c>
       <c r="F18" s="28">

</xml_diff>

<commit_message>
Specification Format Upgrade: Stage 13 - Large scale manual changes to remove/replace those formats that the scripts didn't catch
</commit_message>
<xml_diff>
--- a/readme/XJDF Format Mappings.xlsx
+++ b/readme/XJDF Format Mappings.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="522" uniqueCount="310">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="522" uniqueCount="311">
   <si>
     <t>AnchorFigure</t>
   </si>
@@ -948,6 +948,9 @@
   </si>
   <si>
     <t>Check!</t>
+  </si>
+  <si>
+    <t>SampleCode</t>
   </si>
 </sst>
 </file>
@@ -1577,8 +1580,8 @@
   </sheetPr>
   <dimension ref="B3:E84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="C65" sqref="C65"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="D78" sqref="D78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2386,7 +2389,7 @@
         <v>61</v>
       </c>
       <c r="C71" s="6" t="s">
-        <v>61</v>
+        <v>310</v>
       </c>
       <c r="D71" s="6"/>
       <c r="E71" s="7" t="s">
@@ -2398,7 +2401,7 @@
         <v>62</v>
       </c>
       <c r="C72" s="6" t="s">
-        <v>61</v>
+        <v>310</v>
       </c>
       <c r="D72" s="6"/>
       <c r="E72" s="7"/>
@@ -2408,7 +2411,7 @@
         <v>63</v>
       </c>
       <c r="C73" s="6" t="s">
-        <v>61</v>
+        <v>310</v>
       </c>
       <c r="D73" s="6"/>
       <c r="E73" s="7"/>
@@ -2418,7 +2421,7 @@
         <v>64</v>
       </c>
       <c r="C74" s="6" t="s">
-        <v>61</v>
+        <v>310</v>
       </c>
       <c r="D74" s="6"/>
       <c r="E74" s="7"/>
@@ -2428,7 +2431,7 @@
         <v>65</v>
       </c>
       <c r="C75" s="6" t="s">
-        <v>61</v>
+        <v>310</v>
       </c>
       <c r="D75" s="6"/>
       <c r="E75" s="7"/>
@@ -2438,7 +2441,7 @@
         <v>66</v>
       </c>
       <c r="C76" s="6" t="s">
-        <v>61</v>
+        <v>310</v>
       </c>
       <c r="D76" s="6"/>
       <c r="E76" s="7"/>
@@ -2448,7 +2451,7 @@
         <v>67</v>
       </c>
       <c r="C77" s="6" t="s">
-        <v>61</v>
+        <v>310</v>
       </c>
       <c r="D77" s="6"/>
       <c r="E77" s="7"/>
@@ -2458,7 +2461,7 @@
         <v>68</v>
       </c>
       <c r="C78" s="6" t="s">
-        <v>61</v>
+        <v>310</v>
       </c>
       <c r="D78" s="6"/>
       <c r="E78" s="7"/>
@@ -2468,7 +2471,7 @@
         <v>69</v>
       </c>
       <c r="C79" s="6" t="s">
-        <v>61</v>
+        <v>310</v>
       </c>
       <c r="D79" s="6"/>
       <c r="E79" s="7"/>
@@ -2478,7 +2481,7 @@
         <v>70</v>
       </c>
       <c r="C80" s="6" t="s">
-        <v>61</v>
+        <v>310</v>
       </c>
       <c r="D80" s="6"/>
       <c r="E80" s="7"/>
@@ -2488,7 +2491,7 @@
         <v>71</v>
       </c>
       <c r="C81" s="6" t="s">
-        <v>61</v>
+        <v>310</v>
       </c>
       <c r="D81" s="6"/>
       <c r="E81" s="7"/>
@@ -2498,7 +2501,7 @@
         <v>72</v>
       </c>
       <c r="C82" s="6" t="s">
-        <v>61</v>
+        <v>310</v>
       </c>
       <c r="D82" s="6"/>
       <c r="E82" s="7"/>
@@ -2508,7 +2511,7 @@
         <v>73</v>
       </c>
       <c r="C83" s="6" t="s">
-        <v>61</v>
+        <v>310</v>
       </c>
       <c r="D83" s="6"/>
       <c r="E83" s="7"/>

</xml_diff>